<commit_message>
nested logit log likelihood updated to handle zeros
</commit_message>
<xml_diff>
--- a/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
+++ b/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="with_zeros" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="csv_zeros" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t xml:space="preserve">J / iota</t>
   </si>
@@ -127,6 +129,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,15 +152,17 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +185,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF729FCF"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -297,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -406,6 +417,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,11 +500,11 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -1725,10 +1740,10 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1874,6 +1889,1431 @@
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">Sheet1!E9</f>
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R46"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <f aca="false">SUM(C2:E9)</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <f aca="false">C2*2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <f aca="false">D2+1</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">SUM(L5:N7)</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <f aca="false">C3*2</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <f aca="false">D3+1</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <f aca="false">C4*2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <f aca="false">D4+1</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <f aca="false">C5*2</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <f aca="false">D5+1</f>
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <f aca="false">SUM(C2:C4)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="9" t="n">
+        <f aca="false">SUM(D2:D4)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="10" t="n">
+        <f aca="false">SUM(E2:E4)</f>
+        <v>3</v>
+      </c>
+      <c r="P5" s="0" t="e">
+        <f aca="false">LN(L5)*3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q5" s="0" t="e">
+        <f aca="false">LN(M5)*3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">LN(N5)*3</f>
+        <v>3.29583686600433</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <f aca="false">C6*2</f>
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <f aca="false">D6+1</f>
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="11" t="n">
+        <f aca="false">SUM(C5:C8)</f>
+        <v>22</v>
+      </c>
+      <c r="M6" s="12" t="n">
+        <f aca="false">SUM(D5:D8)</f>
+        <v>44</v>
+      </c>
+      <c r="N6" s="13" t="n">
+        <f aca="false">SUM(E5:E8)</f>
+        <v>48</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <f aca="false">LN(L6)*4</f>
+        <v>12.3641698134333</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <f aca="false">LN(M6)*4</f>
+        <v>15.136758535673</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <f aca="false">LN(N6)*4</f>
+        <v>15.4848040436316</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <f aca="false">C7*2</f>
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <f aca="false">D7+1</f>
+        <v>13</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" s="14" t="n">
+        <f aca="false">C9</f>
+        <v>8</v>
+      </c>
+      <c r="M7" s="15" t="n">
+        <f aca="false">D9</f>
+        <v>16</v>
+      </c>
+      <c r="N7" s="16" t="n">
+        <f aca="false">E9</f>
+        <v>17</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <f aca="false">LN(L7)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <f aca="false">LN(M7)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <f aca="false">LN(N7)</f>
+        <v>2.83321334405622</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <f aca="false">C8*2</f>
+        <v>14</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <f aca="false">D8+1</f>
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="18" t="n">
+        <f aca="false">C9*2</f>
+        <v>16</v>
+      </c>
+      <c r="E9" s="19" t="n">
+        <f aca="false">D9+1</f>
+        <v>17</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="21" t="e">
+        <f aca="false">LN(C2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" s="21" t="e">
+        <f aca="false">LN(D2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="21" t="n">
+        <f aca="false">LN(E2)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="12" t="n">
+        <f aca="false">L5</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="12" t="n">
+        <f aca="false">M5</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="12" t="n">
+        <f aca="false">N5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="21" t="e">
+        <f aca="false">LN(C3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" s="21" t="e">
+        <f aca="false">LN(D3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E13" s="21" t="n">
+        <f aca="false">LN(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="23" t="e">
+        <f aca="false">SUM(C12:E19)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" s="12" t="n">
+        <f aca="false">L12</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="12" t="n">
+        <f aca="false">M12</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="12" t="n">
+        <f aca="false">N12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="21" t="e">
+        <f aca="false">LN(C4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" s="21" t="e">
+        <f aca="false">LN(D4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="21" t="n">
+        <f aca="false">LN(E4)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="27" t="n">
+        <f aca="false">SUM(C15:E19)</f>
+        <v>33.7927555225887</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" s="12" t="n">
+        <f aca="false">L13</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="12" t="n">
+        <f aca="false">M13</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="12" t="n">
+        <f aca="false">N13</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="21" t="n">
+        <f aca="false">LN(C5)</f>
+        <v>1.38629436111989</v>
+      </c>
+      <c r="D15" s="21" t="n">
+        <f aca="false">LN(D5)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="E15" s="21" t="n">
+        <f aca="false">LN(E5)</f>
+        <v>2.19722457733622</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L15" s="12" t="n">
+        <f aca="false">L6</f>
+        <v>22</v>
+      </c>
+      <c r="M15" s="12" t="n">
+        <f aca="false">M6</f>
+        <v>44</v>
+      </c>
+      <c r="N15" s="12" t="n">
+        <f aca="false">N6</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="21" t="n">
+        <f aca="false">LN(C6)</f>
+        <v>1.6094379124341</v>
+      </c>
+      <c r="D16" s="21" t="n">
+        <f aca="false">LN(D6)</f>
+        <v>2.30258509299405</v>
+      </c>
+      <c r="E16" s="21" t="n">
+        <f aca="false">LN(E6)</f>
+        <v>2.39789527279837</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L16" s="12" t="n">
+        <f aca="false">L15</f>
+        <v>22</v>
+      </c>
+      <c r="M16" s="12" t="n">
+        <f aca="false">M15</f>
+        <v>44</v>
+      </c>
+      <c r="N16" s="12" t="n">
+        <f aca="false">N15</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="21" t="n">
+        <f aca="false">LN(C7)</f>
+        <v>1.79175946922806</v>
+      </c>
+      <c r="D17" s="21" t="n">
+        <f aca="false">LN(D7)</f>
+        <v>2.484906649788</v>
+      </c>
+      <c r="E17" s="21" t="n">
+        <f aca="false">LN(E7)</f>
+        <v>2.56494935746154</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L17" s="12" t="n">
+        <f aca="false">L16</f>
+        <v>22</v>
+      </c>
+      <c r="M17" s="12" t="n">
+        <f aca="false">M16</f>
+        <v>44</v>
+      </c>
+      <c r="N17" s="12" t="n">
+        <f aca="false">N16</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="21" t="n">
+        <f aca="false">LN(C8)</f>
+        <v>1.94591014905531</v>
+      </c>
+      <c r="D18" s="21" t="n">
+        <f aca="false">LN(D8)</f>
+        <v>2.63905732961526</v>
+      </c>
+      <c r="E18" s="21" t="n">
+        <f aca="false">LN(E8)</f>
+        <v>2.70805020110221</v>
+      </c>
+      <c r="G18" s="25" t="e">
+        <f aca="false">G13+G25+G32</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L18" s="12" t="n">
+        <f aca="false">L17</f>
+        <v>22</v>
+      </c>
+      <c r="M18" s="12" t="n">
+        <f aca="false">M17</f>
+        <v>44</v>
+      </c>
+      <c r="N18" s="12" t="n">
+        <f aca="false">N17</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="21" t="n">
+        <f aca="false">LN(C9)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="D19" s="21" t="n">
+        <f aca="false">LN(D9)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="E19" s="21" t="n">
+        <f aca="false">LN(E9)</f>
+        <v>2.83321334405622</v>
+      </c>
+      <c r="G19" s="27" t="n">
+        <f aca="false">SUM(G14,G27,H34)</f>
+        <v>293.763641336688</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" s="12" t="n">
+        <f aca="false">L7</f>
+        <v>8</v>
+      </c>
+      <c r="M19" s="12" t="n">
+        <f aca="false">M7</f>
+        <v>16</v>
+      </c>
+      <c r="N19" s="12" t="n">
+        <f aca="false">N7</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="J21" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="21" t="e">
+        <f aca="false">LN(L12)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M23" s="21" t="e">
+        <f aca="false">LN(M12)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N23" s="21" t="n">
+        <f aca="false">LN(N12)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="K24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L24" s="21" t="e">
+        <f aca="false">LN(L13)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M24" s="21" t="e">
+        <f aca="false">LN(M13)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N24" s="21" t="n">
+        <f aca="false">LN(N13)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="23" t="e">
+        <f aca="false">SUM(L23:N30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" s="21" t="e">
+        <f aca="false">LN(L14)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M25" s="21" t="e">
+        <f aca="false">LN(M14)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N25" s="21" t="n">
+        <f aca="false">LN(N14)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="26" t="e">
+        <f aca="false">SUM(P5:R7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L26" s="21" t="n">
+        <f aca="false">LN(L15)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M26" s="21" t="n">
+        <f aca="false">LN(M15)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N26" s="21" t="n">
+        <f aca="false">LN(N15)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="27" t="n">
+        <f aca="false">SUM(P6:R7,R5)</f>
+        <v>53.966812866718</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L27" s="21" t="n">
+        <f aca="false">LN(L16)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M27" s="21" t="n">
+        <f aca="false">LN(M16)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N27" s="21" t="n">
+        <f aca="false">LN(N16)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L28" s="21" t="n">
+        <f aca="false">LN(L17)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M28" s="21" t="n">
+        <f aca="false">LN(M17)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N28" s="21" t="n">
+        <f aca="false">LN(N17)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="n">
+        <f aca="false">L12^2</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">M12^2</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <f aca="false">N12^2</f>
+        <v>9</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L29" s="21" t="n">
+        <f aca="false">LN(L18)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M29" s="21" t="n">
+        <f aca="false">LN(M18)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N29" s="21" t="n">
+        <f aca="false">LN(N18)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="n">
+        <f aca="false">L13^2</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">M13^2</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <f aca="false">N13^2</f>
+        <v>9</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L30" s="21" t="n">
+        <f aca="false">LN(L19)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="M30" s="21" t="n">
+        <f aca="false">LN(M19)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="N30" s="21" t="n">
+        <f aca="false">LN(N19)</f>
+        <v>2.83321334405622</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="n">
+        <f aca="false">L14^2</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">M14^2</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">N14^2</f>
+        <v>9</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="n">
+        <f aca="false">L15^2</f>
+        <v>484</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="false">M15^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <f aca="false">N15^2</f>
+        <v>2304</v>
+      </c>
+      <c r="G32" s="23" t="n">
+        <f aca="false">SUM(H39:J46)</f>
+        <v>206.004072947381</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="n">
+        <f aca="false">L16^2</f>
+        <v>484</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <f aca="false">M16^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <f aca="false">N16^2</f>
+        <v>2304</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="26" t="n">
+        <f aca="false">SUM(H39:J39)*8</f>
+        <v>206.004072947381</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="n">
+        <f aca="false">L17^2</f>
+        <v>484</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">M17^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <f aca="false">N17^2</f>
+        <v>2304</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="27" t="n">
+        <f aca="false">SUM(P38:R38)*8</f>
+        <v>206.004072947381</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="P34" s="0" t="n">
+        <f aca="false">L5^2*3</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <f aca="false">M5^2*3</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <f aca="false">N5^2*3</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="n">
+        <f aca="false">L18^2</f>
+        <v>484</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">M18^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <f aca="false">N18^2</f>
+        <v>2304</v>
+      </c>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="P35" s="1" t="n">
+        <f aca="false">L6^2*4</f>
+        <v>1936</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <f aca="false">M6^2*4</f>
+        <v>7744</v>
+      </c>
+      <c r="R35" s="1" t="n">
+        <f aca="false">N6^2*4</f>
+        <v>9216</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="n">
+        <f aca="false">L19^2</f>
+        <v>64</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">M19^2</f>
+        <v>256</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">N19^2</f>
+        <v>289</v>
+      </c>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="P36" s="1" t="n">
+        <f aca="false">L7^2</f>
+        <v>64</v>
+      </c>
+      <c r="Q36" s="1" t="n">
+        <f aca="false">M7^2</f>
+        <v>256</v>
+      </c>
+      <c r="R36" s="1" t="n">
+        <f aca="false">N7^2</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="P38" s="0" t="n">
+        <f aca="false">LN(SUM(P34:P36))</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <f aca="false">LN(SUM(Q34:Q36))</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="R38" s="1" t="n">
+        <f aca="false">LN(SUM(R34:R36))</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="26" t="n">
+        <f aca="false">LN(C39)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I39" s="26" t="n">
+        <f aca="false">LN(D39)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J39" s="26" t="n">
+        <f aca="false">LN(E39)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" s="26" t="n">
+        <f aca="false">LN(C40)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I40" s="26" t="n">
+        <f aca="false">LN(D40)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J40" s="26" t="n">
+        <f aca="false">LN(E40)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H41" s="26" t="n">
+        <f aca="false">LN(C41)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I41" s="26" t="n">
+        <f aca="false">LN(D41)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J41" s="26" t="n">
+        <f aca="false">LN(E41)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" s="26" t="n">
+        <f aca="false">LN(C42)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I42" s="26" t="n">
+        <f aca="false">LN(D42)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J42" s="26" t="n">
+        <f aca="false">LN(E42)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H43" s="26" t="n">
+        <f aca="false">LN(C43)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I43" s="26" t="n">
+        <f aca="false">LN(D43)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J43" s="26" t="n">
+        <f aca="false">LN(E43)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H44" s="26" t="n">
+        <f aca="false">LN(C44)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I44" s="26" t="n">
+        <f aca="false">LN(D44)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J44" s="26" t="n">
+        <f aca="false">LN(E44)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H45" s="26" t="n">
+        <f aca="false">LN(C45)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I45" s="26" t="n">
+        <f aca="false">LN(D45)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J45" s="26" t="n">
+        <f aca="false">LN(E45)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H46" s="26" t="n">
+        <f aca="false">LN(C46)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I46" s="26" t="n">
+        <f aca="false">LN(D46)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J46" s="26" t="n">
+        <f aca="false">LN(E46)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <f aca="false">with_zeros!C2</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <f aca="false">with_zeros!D2</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <f aca="false">with_zeros!E2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <f aca="false">with_zeros!C3</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <f aca="false">with_zeros!D3</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">with_zeros!E3</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <f aca="false">with_zeros!C4</f>
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <f aca="false">with_zeros!D4</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">with_zeros!E4</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <f aca="false">with_zeros!C5</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <f aca="false">with_zeros!D5</f>
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">with_zeros!E5</f>
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <f aca="false">with_zeros!C6</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <f aca="false">with_zeros!D6</f>
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">with_zeros!E6</f>
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <f aca="false">with_zeros!C7</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <f aca="false">with_zeros!D7</f>
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">with_zeros!E7</f>
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <f aca="false">with_zeros!C8</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <f aca="false">with_zeros!D8</f>
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">with_zeros!E8</f>
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <f aca="false">with_zeros!C9</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <f aca="false">with_zeros!D9</f>
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">with_zeros!E9</f>
         <v>17</v>
       </c>
       <c r="D9" s="5" t="n">

</xml_diff>

<commit_message>
Fixing the nested logit MLE now to be computed with torch elements
</commit_message>
<xml_diff>
--- a/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
+++ b/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="regular" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="csv" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="with_zeros" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="csv_zeros" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -308,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,6 +417,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,11 +504,11 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -1743,7 +1747,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1761,15 +1765,15 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <f aca="false">Sheet1!C2</f>
+        <f aca="false">regular!C2</f>
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <f aca="false">Sheet1!D2</f>
+        <f aca="false">regular!D2</f>
         <v>2</v>
       </c>
       <c r="C2" s="2" t="n">
-        <f aca="false">Sheet1!E2</f>
+        <f aca="false">regular!E2</f>
         <v>3</v>
       </c>
       <c r="D2" s="5" t="n">
@@ -1778,15 +1782,15 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <f aca="false">Sheet1!C3</f>
+        <f aca="false">regular!C3</f>
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <f aca="false">Sheet1!D3</f>
+        <f aca="false">regular!D3</f>
         <v>4</v>
       </c>
       <c r="C3" s="2" t="n">
-        <f aca="false">Sheet1!E3</f>
+        <f aca="false">regular!E3</f>
         <v>5</v>
       </c>
       <c r="D3" s="5" t="n">
@@ -1795,15 +1799,15 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <f aca="false">Sheet1!C4</f>
+        <f aca="false">regular!C4</f>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <f aca="false">Sheet1!D4</f>
+        <f aca="false">regular!D4</f>
         <v>6</v>
       </c>
       <c r="C4" s="2" t="n">
-        <f aca="false">Sheet1!E4</f>
+        <f aca="false">regular!E4</f>
         <v>7</v>
       </c>
       <c r="D4" s="5" t="n">
@@ -1812,15 +1816,15 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <f aca="false">Sheet1!C5</f>
+        <f aca="false">regular!C5</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <f aca="false">Sheet1!D5</f>
+        <f aca="false">regular!D5</f>
         <v>8</v>
       </c>
       <c r="C5" s="2" t="n">
-        <f aca="false">Sheet1!E5</f>
+        <f aca="false">regular!E5</f>
         <v>9</v>
       </c>
       <c r="D5" s="5" t="n">
@@ -1829,15 +1833,15 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <f aca="false">Sheet1!C6</f>
+        <f aca="false">regular!C6</f>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <f aca="false">Sheet1!D6</f>
+        <f aca="false">regular!D6</f>
         <v>10</v>
       </c>
       <c r="C6" s="2" t="n">
-        <f aca="false">Sheet1!E6</f>
+        <f aca="false">regular!E6</f>
         <v>11</v>
       </c>
       <c r="D6" s="5" t="n">
@@ -1846,15 +1850,15 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <f aca="false">Sheet1!C7</f>
+        <f aca="false">regular!C7</f>
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <f aca="false">Sheet1!D7</f>
+        <f aca="false">regular!D7</f>
         <v>12</v>
       </c>
       <c r="C7" s="2" t="n">
-        <f aca="false">Sheet1!E7</f>
+        <f aca="false">regular!E7</f>
         <v>13</v>
       </c>
       <c r="D7" s="5" t="n">
@@ -1863,15 +1867,15 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <f aca="false">Sheet1!C8</f>
+        <f aca="false">regular!C8</f>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <f aca="false">Sheet1!D8</f>
+        <f aca="false">regular!D8</f>
         <v>14</v>
       </c>
       <c r="C8" s="2" t="n">
-        <f aca="false">Sheet1!E8</f>
+        <f aca="false">regular!E8</f>
         <v>15</v>
       </c>
       <c r="D8" s="5" t="n">
@@ -1880,15 +1884,15 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <f aca="false">Sheet1!C9</f>
+        <f aca="false">regular!C9</f>
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <f aca="false">Sheet1!D9</f>
+        <f aca="false">regular!D9</f>
         <v>16</v>
       </c>
       <c r="C9" s="2" t="n">
-        <f aca="false">Sheet1!E9</f>
+        <f aca="false">regular!E9</f>
         <v>17</v>
       </c>
       <c r="D9" s="5" t="n">
@@ -1913,11 +1917,11 @@
   </sheetPr>
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -2068,15 +2072,15 @@
         <f aca="false">SUM(E2:E4)</f>
         <v>3</v>
       </c>
-      <c r="P5" s="0" t="e">
+      <c r="P5" s="26" t="e">
         <f aca="false">LN(L5)*3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q5" s="0" t="e">
+      <c r="Q5" s="26" t="e">
         <f aca="false">LN(M5)*3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="26" t="n">
         <f aca="false">LN(N5)*3</f>
         <v>3.29583686600433</v>
       </c>
@@ -2117,15 +2121,15 @@
         <f aca="false">SUM(E5:E8)</f>
         <v>48</v>
       </c>
-      <c r="P6" s="1" t="n">
+      <c r="P6" s="27" t="n">
         <f aca="false">LN(L6)*4</f>
         <v>12.3641698134333</v>
       </c>
-      <c r="Q6" s="1" t="n">
+      <c r="Q6" s="27" t="n">
         <f aca="false">LN(M6)*4</f>
         <v>15.136758535673</v>
       </c>
-      <c r="R6" s="1" t="n">
+      <c r="R6" s="27" t="n">
         <f aca="false">LN(N6)*4</f>
         <v>15.4848040436316</v>
       </c>
@@ -2163,15 +2167,15 @@
         <f aca="false">E9</f>
         <v>17</v>
       </c>
-      <c r="P7" s="1" t="n">
+      <c r="P7" s="27" t="n">
         <f aca="false">LN(L7)</f>
         <v>2.07944154167984</v>
       </c>
-      <c r="Q7" s="1" t="n">
+      <c r="Q7" s="27" t="n">
         <f aca="false">LN(M7)</f>
         <v>2.77258872223978</v>
       </c>
-      <c r="R7" s="1" t="n">
+      <c r="R7" s="27" t="n">
         <f aca="false">LN(N7)</f>
         <v>2.83321334405622</v>
       </c>
@@ -2194,6 +2198,18 @@
       <c r="G8" s="5" t="n">
         <v>2</v>
       </c>
+      <c r="P8" s="28" t="n">
+        <f aca="false">SUM(P6:P7)</f>
+        <v>14.4436113551131</v>
+      </c>
+      <c r="Q8" s="28" t="n">
+        <f aca="false">SUM(Q6:Q7)</f>
+        <v>17.9093472579128</v>
+      </c>
+      <c r="R8" s="28" t="n">
+        <f aca="false">SUM(R6:R7)+R5</f>
+        <v>21.6138542536921</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
@@ -2218,6 +2234,18 @@
       <c r="J10" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="P10" s="26" t="e">
+        <f aca="false">LN(L5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q10" s="26" t="e">
+        <f aca="false">LN(M5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="26" t="n">
+        <f aca="false">LN(N5)</f>
+        <v>1.09861228866811</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="20" t="s">
@@ -2235,6 +2263,18 @@
       <c r="N11" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="P11" s="26" t="n">
+        <f aca="false">LN(L6)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="Q11" s="26" t="n">
+        <f aca="false">LN(M6)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="R11" s="26" t="n">
+        <f aca="false">LN(N6)</f>
+        <v>3.87120101090789</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -2272,6 +2312,18 @@
       <c r="N12" s="12" t="n">
         <f aca="false">N5</f>
         <v>3</v>
+      </c>
+      <c r="P12" s="26" t="n">
+        <f aca="false">LN(L7)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="Q12" s="26" t="n">
+        <f aca="false">LN(M7)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="R12" s="26" t="n">
+        <f aca="false">LN(N7)</f>
+        <v>2.83321334405622</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,7 +2372,7 @@
         <f aca="false">LN(E4)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="27" t="n">
+      <c r="G14" s="28" t="n">
         <f aca="false">SUM(C15:E19)</f>
         <v>33.7927555225887</v>
       </c>
@@ -2476,7 +2528,7 @@
         <f aca="false">LN(E9)</f>
         <v>2.83321334405622</v>
       </c>
-      <c r="G19" s="27" t="n">
+      <c r="G19" s="28" t="n">
         <f aca="false">SUM(G14,G27,H34)</f>
         <v>293.763641336688</v>
       </c>
@@ -2610,7 +2662,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G27" s="27" t="n">
+      <c r="G27" s="28" t="n">
         <f aca="false">SUM(P6:R7,R5)</f>
         <v>53.966812866718</v>
       </c>
@@ -2785,7 +2837,7 @@
       <c r="G34" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="27" t="n">
+      <c r="H34" s="28" t="n">
         <f aca="false">SUM(P38:R38)*8</f>
         <v>206.004072947381</v>
       </c>
@@ -3168,7 +3220,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
Commiting a more efficient version of the likelihood function for the torch mle, which does operations matrix-wise, orders of magnitude faster than before
</commit_message>
<xml_diff>
--- a/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
+++ b/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
@@ -13,13 +13,14 @@
     <sheet name="regular" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="regular_2" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="csv" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="with_zeros" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="check" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="csv_zeros" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="csv_2" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="with_zeros" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="check" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="csv_zeros" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="53">
   <si>
     <t xml:space="preserve">J / iota</t>
   </si>
@@ -195,12 +196,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -538,7 +538,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -546,13 +546,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -665,7 +665,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,71 +673,71 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,15 +745,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -805,12 +805,12 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Pivot Table Corner" xfId="20"/>
-    <cellStyle name="Pivot Table Value" xfId="21"/>
+    <cellStyle name="Pivot Table Category" xfId="20"/>
+    <cellStyle name="Pivot Table Corner" xfId="21"/>
     <cellStyle name="Pivot Table Field" xfId="22"/>
-    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Result" xfId="23"/>
     <cellStyle name="Pivot Table Title" xfId="24"/>
-    <cellStyle name="Pivot Table Result" xfId="25"/>
+    <cellStyle name="Pivot Table Value" xfId="25"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1009,11 +1009,11 @@
   </sheetPr>
   <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I93" activeCellId="0" sqref="I93:K100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -3936,10 +3936,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="I93:K100 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27"/>
@@ -3968,13 +3968,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="36" t="n">
-        <v>0.364358452837728</v>
+        <v>0.364358452837727</v>
       </c>
       <c r="C3" s="37" t="n">
         <v>0.119762254142615</v>
       </c>
       <c r="D3" s="38" t="n">
-        <v>0.134611228417828</v>
+        <v>0.134611228417827</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4038,10 +4038,10 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L53" activeCellId="1" sqref="I93:K100 L53"/>
+      <selection pane="topLeft" activeCell="L53" activeCellId="0" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -5703,11 +5703,11 @@
   </sheetPr>
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="I93:K100 C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -7382,10 +7382,10 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="I93:K100 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">
@@ -7553,1669 +7553,144 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="I93:K100 F11"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <f aca="false">SUM(C2:E9)</f>
-        <v>158</v>
+      <c r="A1" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="0" t="n">
+        <v>0.36428434</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="51" t="n">
-        <f aca="false">C2*2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="52" t="n">
-        <f aca="false">D2+1</f>
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <f aca="false">SUM(L5:N7)</f>
-        <v>158</v>
+        <v>0.5420817</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.7334709</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
+      <c r="A3" s="0" t="n">
+        <v>0.7077877</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <f aca="false">C3*2</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="54" t="n">
-        <f aca="false">D3+1</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="n">
+        <v>0.39750874</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.7127721</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0.3264838</v>
+      </c>
       <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <f aca="false">C4*2</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="54" t="n">
-        <f aca="false">D4+1</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>3</v>
+        <v>0.41503942</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.79577976</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
+      <c r="A5" s="0" t="n">
+        <v>0.66611</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="53" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <f aca="false">C5*2</f>
-        <v>8</v>
-      </c>
-      <c r="E5" s="54" t="n">
-        <f aca="false">D5+1</f>
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <f aca="false">SUM(C2:C4)</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="4" t="n">
-        <f aca="false">SUM(D2:D4)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="5" t="n">
-        <f aca="false">SUM(E2:E4)</f>
-        <v>3</v>
-      </c>
-      <c r="P5" s="18" t="e">
-        <f aca="false">LN(L5)*3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q5" s="18" t="e">
-        <f aca="false">LN(M5)*3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R5" s="18" t="n">
-        <f aca="false">LN(N5)*3</f>
-        <v>3.29583686600433</v>
+        <v>0.34309506</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.22890705</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
+      <c r="A6" s="0" t="n">
+        <v>0.07764506</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="53" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <f aca="false">C6*2</f>
-        <v>10</v>
-      </c>
-      <c r="E6" s="54" t="n">
-        <f aca="false">D6+1</f>
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" s="6" t="n">
-        <f aca="false">SUM(C5:C8)</f>
-        <v>22</v>
-      </c>
-      <c r="M6" s="7" t="n">
-        <f aca="false">SUM(D5:D8)</f>
-        <v>44</v>
-      </c>
-      <c r="N6" s="8" t="n">
-        <f aca="false">SUM(E5:E8)</f>
-        <v>48</v>
-      </c>
-      <c r="P6" s="59" t="n">
-        <f aca="false">LN(L6)*4</f>
-        <v>12.3641698134333</v>
-      </c>
-      <c r="Q6" s="59" t="n">
-        <f aca="false">LN(M6)*4</f>
-        <v>15.136758535673</v>
-      </c>
-      <c r="R6" s="59" t="n">
-        <f aca="false">LN(N6)*4</f>
-        <v>15.4848040436316</v>
+        <v>0.3604287</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.15933043</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0.08693141</v>
+      </c>
       <c r="B7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" s="53" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <f aca="false">C7*2</f>
-        <v>12</v>
-      </c>
-      <c r="E7" s="54" t="n">
-        <f aca="false">D7+1</f>
-        <v>13</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L7" s="9" t="n">
-        <f aca="false">C9</f>
-        <v>8</v>
-      </c>
-      <c r="M7" s="10" t="n">
-        <f aca="false">D9</f>
-        <v>16</v>
-      </c>
-      <c r="N7" s="11" t="n">
-        <f aca="false">E9</f>
-        <v>17</v>
-      </c>
-      <c r="P7" s="59" t="n">
-        <f aca="false">LN(L7)</f>
-        <v>2.07944154167984</v>
-      </c>
-      <c r="Q7" s="59" t="n">
-        <f aca="false">LN(M7)</f>
-        <v>2.77258872223978</v>
-      </c>
-      <c r="R7" s="59" t="n">
-        <f aca="false">LN(N7)</f>
-        <v>2.83321334405622</v>
+        <v>0.30365914</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.4128874</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0.41172516</v>
+      </c>
       <c r="B8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" s="53" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <f aca="false">C8*2</f>
-        <v>14</v>
-      </c>
-      <c r="E8" s="54" t="n">
-        <f aca="false">D8+1</f>
-        <v>15</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P8" s="58" t="n">
-        <f aca="false">SUM(P6:P7)</f>
-        <v>14.4436113551131</v>
-      </c>
-      <c r="Q8" s="58" t="n">
-        <f aca="false">SUM(Q6:Q7)</f>
-        <v>17.9093472579128</v>
-      </c>
-      <c r="R8" s="58" t="n">
-        <f aca="false">SUM(R6:R7)+R5</f>
-        <v>21.6138542536921</v>
+        <v>0.9873587</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.42125005</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>0.2818082</v>
+      </c>
       <c r="B9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" s="55" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" s="56" t="n">
-        <f aca="false">C9*2</f>
-        <v>16</v>
-      </c>
-      <c r="E9" s="57" t="n">
-        <f aca="false">D9+1</f>
-        <v>17</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="P10" s="18" t="e">
-        <f aca="false">LN(L5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q10" s="18" t="e">
-        <f aca="false">LN(M5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R10" s="18" t="n">
-        <f aca="false">LN(N5)</f>
-        <v>1.09861228866811</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P11" s="18" t="n">
-        <f aca="false">LN(L6)</f>
-        <v>3.09104245335832</v>
-      </c>
-      <c r="Q11" s="18" t="n">
-        <f aca="false">LN(M6)</f>
-        <v>3.78418963391826</v>
-      </c>
-      <c r="R11" s="18" t="n">
-        <f aca="false">LN(N6)</f>
-        <v>3.87120101090789</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="13" t="e">
-        <f aca="false">LN(C2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" s="13" t="e">
-        <f aca="false">LN(D2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E12" s="13" t="n">
-        <f aca="false">LN(E2)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="7" t="n">
-        <f aca="false">L5</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="7" t="n">
-        <f aca="false">M5</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="7" t="n">
-        <f aca="false">N5</f>
-        <v>3</v>
-      </c>
-      <c r="P12" s="18" t="n">
-        <f aca="false">LN(L7)</f>
-        <v>2.07944154167984</v>
-      </c>
-      <c r="Q12" s="18" t="n">
-        <f aca="false">LN(M7)</f>
-        <v>2.77258872223978</v>
-      </c>
-      <c r="R12" s="18" t="n">
-        <f aca="false">LN(N7)</f>
-        <v>2.83321334405622</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="13" t="e">
-        <f aca="false">LN(C3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" s="13" t="e">
-        <f aca="false">LN(D3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E13" s="13" t="n">
-        <f aca="false">LN(E3)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="15" t="e">
-        <f aca="false">SUM(C12:E19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="n">
-        <f aca="false">L12</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="7" t="n">
-        <f aca="false">M12</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="7" t="n">
-        <f aca="false">N12</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="13" t="e">
-        <f aca="false">LN(C4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D14" s="13" t="e">
-        <f aca="false">LN(D4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E14" s="13" t="n">
-        <f aca="false">LN(E4)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="58" t="n">
-        <f aca="false">SUM(C15:E19)</f>
-        <v>33.7927555225887</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L14" s="7" t="n">
-        <f aca="false">L13</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="7" t="n">
-        <f aca="false">M13</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="7" t="n">
-        <f aca="false">N13</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="13" t="n">
-        <f aca="false">LN(C5)</f>
-        <v>1.38629436111989</v>
-      </c>
-      <c r="D15" s="13" t="n">
-        <f aca="false">LN(D5)</f>
-        <v>2.07944154167984</v>
-      </c>
-      <c r="E15" s="13" t="n">
-        <f aca="false">LN(E5)</f>
-        <v>2.19722457733622</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L15" s="7" t="n">
-        <f aca="false">L6</f>
-        <v>22</v>
-      </c>
-      <c r="M15" s="7" t="n">
-        <f aca="false">M6</f>
-        <v>44</v>
-      </c>
-      <c r="N15" s="7" t="n">
-        <f aca="false">N6</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="13" t="n">
-        <f aca="false">LN(C6)</f>
-        <v>1.6094379124341</v>
-      </c>
-      <c r="D16" s="13" t="n">
-        <f aca="false">LN(D6)</f>
-        <v>2.30258509299405</v>
-      </c>
-      <c r="E16" s="13" t="n">
-        <f aca="false">LN(E6)</f>
-        <v>2.39789527279837</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L16" s="7" t="n">
-        <f aca="false">L15</f>
-        <v>22</v>
-      </c>
-      <c r="M16" s="7" t="n">
-        <f aca="false">M15</f>
-        <v>44</v>
-      </c>
-      <c r="N16" s="7" t="n">
-        <f aca="false">N15</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="13" t="n">
-        <f aca="false">LN(C7)</f>
-        <v>1.79175946922806</v>
-      </c>
-      <c r="D17" s="13" t="n">
-        <f aca="false">LN(D7)</f>
-        <v>2.484906649788</v>
-      </c>
-      <c r="E17" s="13" t="n">
-        <f aca="false">LN(E7)</f>
-        <v>2.56494935746154</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L17" s="7" t="n">
-        <f aca="false">L16</f>
-        <v>22</v>
-      </c>
-      <c r="M17" s="7" t="n">
-        <f aca="false">M16</f>
-        <v>44</v>
-      </c>
-      <c r="N17" s="7" t="n">
-        <f aca="false">N16</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="13" t="n">
-        <f aca="false">LN(C8)</f>
-        <v>1.94591014905531</v>
-      </c>
-      <c r="D18" s="13" t="n">
-        <f aca="false">LN(D8)</f>
-        <v>2.63905732961526</v>
-      </c>
-      <c r="E18" s="13" t="n">
-        <f aca="false">LN(E8)</f>
-        <v>2.70805020110221</v>
-      </c>
-      <c r="G18" s="17" t="e">
-        <f aca="false">G13+G25+G32</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L18" s="7" t="n">
-        <f aca="false">L17</f>
-        <v>22</v>
-      </c>
-      <c r="M18" s="7" t="n">
-        <f aca="false">M17</f>
-        <v>44</v>
-      </c>
-      <c r="N18" s="7" t="n">
-        <f aca="false">N17</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="13" t="n">
-        <f aca="false">LN(C9)</f>
-        <v>2.07944154167984</v>
-      </c>
-      <c r="D19" s="13" t="n">
-        <f aca="false">LN(D9)</f>
-        <v>2.77258872223978</v>
-      </c>
-      <c r="E19" s="13" t="n">
-        <f aca="false">LN(E9)</f>
-        <v>2.83321334405622</v>
-      </c>
-      <c r="G19" s="58" t="n">
-        <f aca="false">G14+G27-H34</f>
-        <v>-118.244504558075</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L19" s="7" t="n">
-        <f aca="false">L7</f>
-        <v>8</v>
-      </c>
-      <c r="M19" s="7" t="n">
-        <f aca="false">M7</f>
-        <v>16</v>
-      </c>
-      <c r="N19" s="7" t="n">
-        <f aca="false">N7</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="J21" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="L22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M22" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N22" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" s="13" t="e">
-        <f aca="false">LN(L12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M23" s="13" t="e">
-        <f aca="false">LN(M12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N23" s="13" t="n">
-        <f aca="false">LN(N12)</f>
-        <v>1.09861228866811</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G24" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="14"/>
-      <c r="K24" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L24" s="13" t="e">
-        <f aca="false">LN(L13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M24" s="13" t="e">
-        <f aca="false">LN(M13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N24" s="13" t="n">
-        <f aca="false">LN(N13)</f>
-        <v>1.09861228866811</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="15" t="e">
-        <f aca="false">SUM(L23:N30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L25" s="13" t="e">
-        <f aca="false">LN(L14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M25" s="13" t="e">
-        <f aca="false">LN(M14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N25" s="13" t="n">
-        <f aca="false">LN(N14)</f>
-        <v>1.09861228866811</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="18" t="e">
-        <f aca="false">SUM(P5:R7)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L26" s="13" t="n">
-        <f aca="false">LN(L15)</f>
-        <v>3.09104245335832</v>
-      </c>
-      <c r="M26" s="13" t="n">
-        <f aca="false">LN(M15)</f>
-        <v>3.78418963391826</v>
-      </c>
-      <c r="N26" s="13" t="n">
-        <f aca="false">LN(N15)</f>
-        <v>3.87120101090789</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G27" s="58" t="n">
-        <f aca="false">SUM(P6:R7,R5)</f>
-        <v>53.966812866718</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L27" s="13" t="n">
-        <f aca="false">LN(L16)</f>
-        <v>3.09104245335832</v>
-      </c>
-      <c r="M27" s="13" t="n">
-        <f aca="false">LN(M16)</f>
-        <v>3.78418963391826</v>
-      </c>
-      <c r="N27" s="13" t="n">
-        <f aca="false">LN(N16)</f>
-        <v>3.87120101090789</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="L28" s="13" t="n">
-        <f aca="false">LN(L17)</f>
-        <v>3.09104245335832</v>
-      </c>
-      <c r="M28" s="13" t="n">
-        <f aca="false">LN(M17)</f>
-        <v>3.78418963391826</v>
-      </c>
-      <c r="N28" s="13" t="n">
-        <f aca="false">LN(N17)</f>
-        <v>3.87120101090789</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="n">
-        <f aca="false">L12^2</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <f aca="false">M12^2</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="1" t="n">
-        <f aca="false">N12^2</f>
-        <v>9</v>
-      </c>
-      <c r="K29" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="L29" s="13" t="n">
-        <f aca="false">LN(L18)</f>
-        <v>3.09104245335832</v>
-      </c>
-      <c r="M29" s="13" t="n">
-        <f aca="false">LN(M18)</f>
-        <v>3.78418963391826</v>
-      </c>
-      <c r="N29" s="13" t="n">
-        <f aca="false">LN(N18)</f>
-        <v>3.87120101090789</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="n">
-        <f aca="false">L13^2</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <f aca="false">M13^2</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="1" t="n">
-        <f aca="false">N13^2</f>
-        <v>9</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="L30" s="13" t="n">
-        <f aca="false">LN(L19)</f>
-        <v>2.07944154167984</v>
-      </c>
-      <c r="M30" s="13" t="n">
-        <f aca="false">LN(M19)</f>
-        <v>2.77258872223978</v>
-      </c>
-      <c r="N30" s="13" t="n">
-        <f aca="false">LN(N19)</f>
-        <v>2.83321334405622</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="n">
-        <f aca="false">L14^2</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="1" t="n">
-        <f aca="false">M14^2</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="1" t="n">
-        <f aca="false">N14^2</f>
-        <v>9</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="n">
-        <f aca="false">L15^2</f>
-        <v>484</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <f aca="false">M15^2</f>
-        <v>1936</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <f aca="false">N15^2</f>
-        <v>2304</v>
-      </c>
-      <c r="G32" s="15" t="n">
-        <f aca="false">SUM(H39:J46)</f>
-        <v>206.004072947381</v>
-      </c>
-      <c r="L32" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="n">
-        <f aca="false">L16^2</f>
-        <v>484</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <f aca="false">M16^2</f>
-        <v>1936</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <f aca="false">N16^2</f>
-        <v>2304</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="18" t="n">
-        <f aca="false">SUM(H39:J39)*8</f>
-        <v>206.004072947381</v>
-      </c>
-      <c r="L33" s="20" t="e">
-        <f aca="false">check!C2/check!L$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" s="20" t="e">
-        <f aca="false">check!D2/check!M$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N33" s="20" t="n">
-        <f aca="false">check!E2/check!N$5</f>
-        <v>0.333333333333333</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="0" t="n">
-        <f aca="false">L17^2</f>
-        <v>484</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <f aca="false">M17^2</f>
-        <v>1936</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <f aca="false">N17^2</f>
-        <v>2304</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="58" t="n">
-        <f aca="false">SUM(P38:R38)*8</f>
-        <v>206.004072947381</v>
-      </c>
-      <c r="L34" s="20" t="e">
-        <f aca="false">check!C3/check!L$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" s="20" t="e">
-        <f aca="false">check!D3/check!M$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N34" s="20" t="n">
-        <f aca="false">check!E3/check!N$5</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="P34" s="0" t="n">
-        <f aca="false">L5^2*3</f>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="0" t="n">
-        <f aca="false">M5^2*3</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="0" t="n">
-        <f aca="false">N5^2*3</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="0" t="n">
-        <f aca="false">L18^2</f>
-        <v>484</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <f aca="false">M18^2</f>
-        <v>1936</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <f aca="false">N18^2</f>
-        <v>2304</v>
-      </c>
-      <c r="L35" s="20" t="e">
-        <f aca="false">check!C4/check!L$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="20" t="e">
-        <f aca="false">check!D4/check!M$5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N35" s="20" t="n">
-        <f aca="false">check!E4/check!N$5</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="P35" s="1" t="n">
-        <f aca="false">L6^2*4</f>
-        <v>1936</v>
-      </c>
-      <c r="Q35" s="1" t="n">
-        <f aca="false">M6^2*4</f>
-        <v>7744</v>
-      </c>
-      <c r="R35" s="1" t="n">
-        <f aca="false">N6^2*4</f>
-        <v>9216</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="n">
-        <f aca="false">L19^2</f>
-        <v>64</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <f aca="false">M19^2</f>
-        <v>256</v>
-      </c>
-      <c r="E36" s="1" t="n">
-        <f aca="false">N19^2</f>
-        <v>289</v>
-      </c>
-      <c r="L36" s="20" t="n">
-        <f aca="false">check!C5/check!L$6</f>
-        <v>0.181818181818182</v>
-      </c>
-      <c r="M36" s="20" t="n">
-        <f aca="false">check!D5/check!M$6</f>
-        <v>0.181818181818182</v>
-      </c>
-      <c r="N36" s="20" t="n">
-        <f aca="false">check!E5/check!N$6</f>
-        <v>0.1875</v>
-      </c>
-      <c r="P36" s="1" t="n">
-        <f aca="false">L7^2</f>
-        <v>64</v>
-      </c>
-      <c r="Q36" s="1" t="n">
-        <f aca="false">M7^2</f>
-        <v>256</v>
-      </c>
-      <c r="R36" s="1" t="n">
-        <f aca="false">N7^2</f>
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="L37" s="20" t="n">
-        <f aca="false">check!C6/check!L$6</f>
-        <v>0.227272727272727</v>
-      </c>
-      <c r="M37" s="20" t="n">
-        <f aca="false">check!D6/check!M$6</f>
-        <v>0.227272727272727</v>
-      </c>
-      <c r="N37" s="20" t="n">
-        <f aca="false">check!E6/check!N$6</f>
-        <v>0.229166666666667</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="G38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="L38" s="20" t="n">
-        <f aca="false">check!C7/check!L$6</f>
-        <v>0.272727272727273</v>
-      </c>
-      <c r="M38" s="20" t="n">
-        <f aca="false">check!D7/check!M$6</f>
-        <v>0.272727272727273</v>
-      </c>
-      <c r="N38" s="20" t="n">
-        <f aca="false">check!E7/check!N$6</f>
-        <v>0.270833333333333</v>
-      </c>
-      <c r="P38" s="0" t="n">
-        <f aca="false">LN(SUM(P34:P36))</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="Q38" s="1" t="n">
-        <f aca="false">LN(SUM(Q34:Q36))</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="R38" s="1" t="n">
-        <f aca="false">LN(SUM(R34:R36))</f>
-        <v>9.16240983821863</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E39" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H39" s="18" t="n">
-        <f aca="false">LN(C39)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I39" s="18" t="n">
-        <f aca="false">LN(D39)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J39" s="18" t="n">
-        <f aca="false">LN(E39)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L39" s="20" t="n">
-        <f aca="false">check!C8/check!L$6</f>
-        <v>0.318181818181818</v>
-      </c>
-      <c r="M39" s="20" t="n">
-        <f aca="false">check!D8/check!M$6</f>
-        <v>0.318181818181818</v>
-      </c>
-      <c r="N39" s="20" t="n">
-        <f aca="false">check!E8/check!N$6</f>
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G40" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H40" s="18" t="n">
-        <f aca="false">LN(C40)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I40" s="18" t="n">
-        <f aca="false">LN(D40)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J40" s="18" t="n">
-        <f aca="false">LN(E40)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L40" s="20" t="n">
-        <f aca="false">check!C9/check!L$7</f>
-        <v>1</v>
-      </c>
-      <c r="M40" s="20" t="n">
-        <f aca="false">check!D9/check!M$7</f>
-        <v>1</v>
-      </c>
-      <c r="N40" s="20" t="n">
-        <f aca="false">check!E9/check!N$7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H41" s="18" t="n">
-        <f aca="false">LN(C41)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I41" s="18" t="n">
-        <f aca="false">LN(D41)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J41" s="18" t="n">
-        <f aca="false">LN(E41)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="K41" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="L41" s="0" t="n">
-        <f aca="false">SUM(L36:L40)</f>
-        <v>2</v>
-      </c>
-      <c r="M41" s="0" t="n">
-        <f aca="false">SUM(M36:M40)</f>
-        <v>2</v>
-      </c>
-      <c r="N41" s="0" t="n">
-        <f aca="false">SUM(N33:N40)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E42" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G42" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H42" s="18" t="n">
-        <f aca="false">LN(C42)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I42" s="18" t="n">
-        <f aca="false">LN(D42)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J42" s="18" t="n">
-        <f aca="false">LN(E42)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L42" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E43" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G43" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H43" s="18" t="n">
-        <f aca="false">LN(C43)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I43" s="18" t="n">
-        <f aca="false">LN(D43)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J43" s="18" t="n">
-        <f aca="false">LN(E43)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L43" s="19" t="n">
-        <f aca="false">C29/C39</f>
-        <v>0</v>
-      </c>
-      <c r="M43" s="19" t="n">
-        <f aca="false">D29/D39</f>
-        <v>0</v>
-      </c>
-      <c r="N43" s="19" t="n">
-        <f aca="false">E29/E39</f>
-        <v>0.000944187998321444</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E44" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H44" s="18" t="n">
-        <f aca="false">LN(C44)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I44" s="18" t="n">
-        <f aca="false">LN(D44)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J44" s="18" t="n">
-        <f aca="false">LN(E44)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L44" s="19" t="n">
-        <f aca="false">C30/C40</f>
-        <v>0</v>
-      </c>
-      <c r="M44" s="19" t="n">
-        <f aca="false">D30/D40</f>
-        <v>0</v>
-      </c>
-      <c r="N44" s="19" t="n">
-        <f aca="false">E30/E40</f>
-        <v>0.000944187998321444</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D45" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E45" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G45" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H45" s="18" t="n">
-        <f aca="false">LN(C45)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I45" s="18" t="n">
-        <f aca="false">LN(D45)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J45" s="18" t="n">
-        <f aca="false">LN(E45)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L45" s="19" t="n">
-        <f aca="false">C31/C41</f>
-        <v>0</v>
-      </c>
-      <c r="M45" s="19" t="n">
-        <f aca="false">D31/D41</f>
-        <v>0</v>
-      </c>
-      <c r="N45" s="19" t="n">
-        <f aca="false">E31/E41</f>
-        <v>0.000944187998321444</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <f aca="false">SUM(C$29:C$36)</f>
-        <v>2000</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <f aca="false">SUM(D$29:D$36)</f>
-        <v>8000</v>
-      </c>
-      <c r="E46" s="1" t="n">
-        <f aca="false">SUM(E$29:E$36)</f>
-        <v>9532</v>
-      </c>
-      <c r="G46" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H46" s="18" t="n">
-        <f aca="false">LN(C46)</f>
-        <v>7.60090245954208</v>
-      </c>
-      <c r="I46" s="18" t="n">
-        <f aca="false">LN(D46)</f>
-        <v>8.98719682066197</v>
-      </c>
-      <c r="J46" s="18" t="n">
-        <f aca="false">LN(E46)</f>
-        <v>9.16240983821863</v>
-      </c>
-      <c r="L46" s="19" t="n">
-        <f aca="false">C32/C42</f>
-        <v>0.242</v>
-      </c>
-      <c r="M46" s="19" t="n">
-        <f aca="false">D32/D42</f>
-        <v>0.242</v>
-      </c>
-      <c r="N46" s="19" t="n">
-        <f aca="false">E32/E42</f>
-        <v>0.24171212757029</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L47" s="19" t="n">
-        <f aca="false">C33/C43</f>
-        <v>0.242</v>
-      </c>
-      <c r="M47" s="19" t="n">
-        <f aca="false">D33/D43</f>
-        <v>0.242</v>
-      </c>
-      <c r="N47" s="19" t="n">
-        <f aca="false">E33/E43</f>
-        <v>0.24171212757029</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L48" s="19" t="n">
-        <f aca="false">C34/C44</f>
-        <v>0.242</v>
-      </c>
-      <c r="M48" s="19" t="n">
-        <f aca="false">D34/D44</f>
-        <v>0.242</v>
-      </c>
-      <c r="N48" s="19" t="n">
-        <f aca="false">E34/E44</f>
-        <v>0.24171212757029</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L49" s="19" t="n">
-        <f aca="false">C35/C45</f>
-        <v>0.242</v>
-      </c>
-      <c r="M49" s="19" t="n">
-        <f aca="false">D35/D45</f>
-        <v>0.242</v>
-      </c>
-      <c r="N49" s="19" t="n">
-        <f aca="false">E35/E45</f>
-        <v>0.24171212757029</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L50" s="19" t="n">
-        <f aca="false">C36/C46</f>
-        <v>0.032</v>
-      </c>
-      <c r="M50" s="19" t="n">
-        <f aca="false">D36/D46</f>
-        <v>0.032</v>
-      </c>
-      <c r="N50" s="19" t="n">
-        <f aca="false">E36/E46</f>
-        <v>0.0303189257238775</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K51" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="L51" s="0" t="n">
-        <f aca="false">SUM(L46:L50)</f>
-        <v>1</v>
-      </c>
-      <c r="M51" s="0" t="n">
-        <f aca="false">SUM(M46:M50)</f>
-        <v>1</v>
-      </c>
-      <c r="N51" s="0" t="n">
-        <f aca="false">SUM(N43:N50)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L52" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L53" s="24" t="e">
-        <f aca="false">L33*L43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M53" s="24" t="e">
-        <f aca="false">M33*M43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N53" s="24" t="n">
-        <f aca="false">N33*N43</f>
-        <v>0.000314729332773814</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L54" s="24" t="e">
-        <f aca="false">L34*L44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M54" s="24" t="e">
-        <f aca="false">M34*M44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N54" s="24" t="n">
-        <f aca="false">N34*N44</f>
-        <v>0.000314729332773814</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L55" s="24" t="e">
-        <f aca="false">L35*L45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M55" s="24" t="e">
-        <f aca="false">M35*M45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N55" s="24" t="n">
-        <f aca="false">N35*N45</f>
-        <v>0.000314729332773814</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L56" s="24" t="n">
-        <f aca="false">L36*L46</f>
-        <v>0.044</v>
-      </c>
-      <c r="M56" s="24" t="n">
-        <f aca="false">M36*M46</f>
-        <v>0.044</v>
-      </c>
-      <c r="N56" s="24" t="n">
-        <f aca="false">N36*N46</f>
-        <v>0.0453210239194293</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L57" s="24" t="n">
-        <f aca="false">L37*L47</f>
-        <v>0.055</v>
-      </c>
-      <c r="M57" s="24" t="n">
-        <f aca="false">M37*M47</f>
-        <v>0.055</v>
-      </c>
-      <c r="N57" s="24" t="n">
-        <f aca="false">N37*N47</f>
-        <v>0.0553923625681914</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L58" s="24" t="n">
-        <f aca="false">L38*L48</f>
-        <v>0.066</v>
-      </c>
-      <c r="M58" s="24" t="n">
-        <f aca="false">M38*M48</f>
-        <v>0.066</v>
-      </c>
-      <c r="N58" s="24" t="n">
-        <f aca="false">N38*N48</f>
-        <v>0.0654637012169534</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L59" s="24" t="n">
-        <f aca="false">L39*L49</f>
-        <v>0.077</v>
-      </c>
-      <c r="M59" s="24" t="n">
-        <f aca="false">M39*M49</f>
-        <v>0.077</v>
-      </c>
-      <c r="N59" s="24" t="n">
-        <f aca="false">N39*N49</f>
-        <v>0.0755350398657155</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L60" s="24" t="n">
-        <f aca="false">L40*L50</f>
-        <v>0.032</v>
-      </c>
-      <c r="M60" s="24" t="n">
-        <f aca="false">M40*M50</f>
-        <v>0.032</v>
-      </c>
-      <c r="N60" s="24" t="n">
-        <f aca="false">N40*N50</f>
-        <v>0.0303189257238775</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K61" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="L61" s="0" t="n">
-        <f aca="false">SUM(L56:L60)</f>
-        <v>0.274</v>
-      </c>
-      <c r="M61" s="0" t="n">
-        <f aca="false">SUM(M56:M60)</f>
-        <v>0.274</v>
-      </c>
-      <c r="N61" s="0" t="n">
-        <f aca="false">SUM(N53:N60)</f>
-        <v>0.272975241292488</v>
+        <v>0.6199603</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.648762</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9228,13 +7703,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="1" sqref="I93:K100 L34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -10118,6 +8593,11 @@
         <f aca="false">SUM(H39:J46)</f>
         <v>206.004072947381</v>
       </c>
+      <c r="L32" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="n">
@@ -10139,6 +8619,18 @@
         <f aca="false">SUM(H39:J39)*8</f>
         <v>206.004072947381</v>
       </c>
+      <c r="L33" s="20" t="e">
+        <f aca="false">check!C2/check!L$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="20" t="e">
+        <f aca="false">check!D2/check!M$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N33" s="20" t="n">
+        <f aca="false">check!E2/check!N$5</f>
+        <v>0.333333333333333</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="n">
@@ -10160,6 +8652,18 @@
         <f aca="false">SUM(P38:R38)*8</f>
         <v>206.004072947381</v>
       </c>
+      <c r="L34" s="20" t="e">
+        <f aca="false">check!C3/check!L$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34" s="20" t="e">
+        <f aca="false">check!D3/check!M$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N34" s="20" t="n">
+        <f aca="false">check!E3/check!N$5</f>
+        <v>0.333333333333333</v>
+      </c>
       <c r="P34" s="0" t="n">
         <f aca="false">L5^2*3</f>
         <v>0</v>
@@ -10186,6 +8690,18 @@
         <f aca="false">N18^2</f>
         <v>2304</v>
       </c>
+      <c r="L35" s="20" t="e">
+        <f aca="false">check!C4/check!L$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="20" t="e">
+        <f aca="false">check!D4/check!M$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N35" s="20" t="n">
+        <f aca="false">check!E4/check!N$5</f>
+        <v>0.333333333333333</v>
+      </c>
       <c r="P35" s="1" t="n">
         <f aca="false">L6^2*4</f>
         <v>1936</v>
@@ -10212,6 +8728,18 @@
         <f aca="false">N19^2</f>
         <v>289</v>
       </c>
+      <c r="L36" s="20" t="n">
+        <f aca="false">check!C5/check!L$6</f>
+        <v>0.181818181818182</v>
+      </c>
+      <c r="M36" s="20" t="n">
+        <f aca="false">check!D5/check!M$6</f>
+        <v>0.181818181818182</v>
+      </c>
+      <c r="N36" s="20" t="n">
+        <f aca="false">check!E5/check!N$6</f>
+        <v>0.1875</v>
+      </c>
       <c r="P36" s="1" t="n">
         <f aca="false">L7^2</f>
         <v>64</v>
@@ -10228,6 +8756,18 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
+      <c r="L37" s="20" t="n">
+        <f aca="false">check!C6/check!L$6</f>
+        <v>0.227272727272727</v>
+      </c>
+      <c r="M37" s="20" t="n">
+        <f aca="false">check!D6/check!M$6</f>
+        <v>0.227272727272727</v>
+      </c>
+      <c r="N37" s="20" t="n">
+        <f aca="false">check!E6/check!N$6</f>
+        <v>0.229166666666667</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
@@ -10240,6 +8780,18 @@
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
+      <c r="L38" s="20" t="n">
+        <f aca="false">check!C7/check!L$6</f>
+        <v>0.272727272727273</v>
+      </c>
+      <c r="M38" s="20" t="n">
+        <f aca="false">check!D7/check!M$6</f>
+        <v>0.272727272727273</v>
+      </c>
+      <c r="N38" s="20" t="n">
+        <f aca="false">check!E7/check!N$6</f>
+        <v>0.270833333333333</v>
+      </c>
       <c r="P38" s="0" t="n">
         <f aca="false">LN(SUM(P34:P36))</f>
         <v>7.60090245954208</v>
@@ -10284,6 +8836,18 @@
         <f aca="false">LN(E39)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L39" s="20" t="n">
+        <f aca="false">check!C8/check!L$6</f>
+        <v>0.318181818181818</v>
+      </c>
+      <c r="M39" s="20" t="n">
+        <f aca="false">check!D8/check!M$6</f>
+        <v>0.318181818181818</v>
+      </c>
+      <c r="N39" s="20" t="n">
+        <f aca="false">check!E8/check!N$6</f>
+        <v>0.3125</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
@@ -10316,6 +8880,18 @@
         <f aca="false">LN(E40)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L40" s="20" t="n">
+        <f aca="false">check!C9/check!L$7</f>
+        <v>1</v>
+      </c>
+      <c r="M40" s="20" t="n">
+        <f aca="false">check!D9/check!M$7</f>
+        <v>1</v>
+      </c>
+      <c r="N40" s="20" t="n">
+        <f aca="false">check!E9/check!N$7</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="n">
@@ -10348,6 +8924,21 @@
         <f aca="false">LN(E41)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="K41" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <f aca="false">SUM(L36:L40)</f>
+        <v>2</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <f aca="false">SUM(M36:M40)</f>
+        <v>2</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <f aca="false">SUM(N33:N40)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="n">
@@ -10380,6 +8971,11 @@
         <f aca="false">LN(E42)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L42" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="n">
@@ -10412,6 +9008,18 @@
         <f aca="false">LN(E43)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L43" s="19" t="n">
+        <f aca="false">C29/C39</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="19" t="n">
+        <f aca="false">D29/D39</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="19" t="n">
+        <f aca="false">E29/E39</f>
+        <v>0.000944187998321444</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="n">
@@ -10444,6 +9052,18 @@
         <f aca="false">LN(E44)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L44" s="19" t="n">
+        <f aca="false">C30/C40</f>
+        <v>0</v>
+      </c>
+      <c r="M44" s="19" t="n">
+        <f aca="false">D30/D40</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="19" t="n">
+        <f aca="false">E30/E40</f>
+        <v>0.000944187998321444</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="n">
@@ -10476,6 +9096,18 @@
         <f aca="false">LN(E45)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L45" s="19" t="n">
+        <f aca="false">C31/C41</f>
+        <v>0</v>
+      </c>
+      <c r="M45" s="19" t="n">
+        <f aca="false">D31/D41</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="19" t="n">
+        <f aca="false">E31/E41</f>
+        <v>0.000944187998321444</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="n">
@@ -10508,11 +9140,232 @@
         <f aca="false">LN(E46)</f>
         <v>9.16240983821863</v>
       </c>
+      <c r="L46" s="19" t="n">
+        <f aca="false">C32/C42</f>
+        <v>0.242</v>
+      </c>
+      <c r="M46" s="19" t="n">
+        <f aca="false">D32/D42</f>
+        <v>0.242</v>
+      </c>
+      <c r="N46" s="19" t="n">
+        <f aca="false">E32/E42</f>
+        <v>0.24171212757029</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="19" t="n">
+        <f aca="false">C33/C43</f>
+        <v>0.242</v>
+      </c>
+      <c r="M47" s="19" t="n">
+        <f aca="false">D33/D43</f>
+        <v>0.242</v>
+      </c>
+      <c r="N47" s="19" t="n">
+        <f aca="false">E33/E43</f>
+        <v>0.24171212757029</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L48" s="19" t="n">
+        <f aca="false">C34/C44</f>
+        <v>0.242</v>
+      </c>
+      <c r="M48" s="19" t="n">
+        <f aca="false">D34/D44</f>
+        <v>0.242</v>
+      </c>
+      <c r="N48" s="19" t="n">
+        <f aca="false">E34/E44</f>
+        <v>0.24171212757029</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L49" s="19" t="n">
+        <f aca="false">C35/C45</f>
+        <v>0.242</v>
+      </c>
+      <c r="M49" s="19" t="n">
+        <f aca="false">D35/D45</f>
+        <v>0.242</v>
+      </c>
+      <c r="N49" s="19" t="n">
+        <f aca="false">E35/E45</f>
+        <v>0.24171212757029</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L50" s="19" t="n">
+        <f aca="false">C36/C46</f>
+        <v>0.032</v>
+      </c>
+      <c r="M50" s="19" t="n">
+        <f aca="false">D36/D46</f>
+        <v>0.032</v>
+      </c>
+      <c r="N50" s="19" t="n">
+        <f aca="false">E36/E46</f>
+        <v>0.0303189257238775</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K51" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="0" t="n">
+        <f aca="false">SUM(L46:L50)</f>
+        <v>1</v>
+      </c>
+      <c r="M51" s="0" t="n">
+        <f aca="false">SUM(M46:M50)</f>
+        <v>1</v>
+      </c>
+      <c r="N51" s="0" t="n">
+        <f aca="false">SUM(N43:N50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L52" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="24"/>
+      <c r="N52" s="24"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L53" s="24" t="e">
+        <f aca="false">L33*L43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M53" s="24" t="e">
+        <f aca="false">M33*M43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N53" s="24" t="n">
+        <f aca="false">N33*N43</f>
+        <v>0.000314729332773814</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L54" s="24" t="e">
+        <f aca="false">L34*L44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M54" s="24" t="e">
+        <f aca="false">M34*M44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N54" s="24" t="n">
+        <f aca="false">N34*N44</f>
+        <v>0.000314729332773814</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L55" s="24" t="e">
+        <f aca="false">L35*L45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M55" s="24" t="e">
+        <f aca="false">M35*M45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N55" s="24" t="n">
+        <f aca="false">N35*N45</f>
+        <v>0.000314729332773814</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L56" s="24" t="n">
+        <f aca="false">L36*L46</f>
+        <v>0.044</v>
+      </c>
+      <c r="M56" s="24" t="n">
+        <f aca="false">M36*M46</f>
+        <v>0.044</v>
+      </c>
+      <c r="N56" s="24" t="n">
+        <f aca="false">N36*N46</f>
+        <v>0.0453210239194293</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L57" s="24" t="n">
+        <f aca="false">L37*L47</f>
+        <v>0.055</v>
+      </c>
+      <c r="M57" s="24" t="n">
+        <f aca="false">M37*M47</f>
+        <v>0.055</v>
+      </c>
+      <c r="N57" s="24" t="n">
+        <f aca="false">N37*N47</f>
+        <v>0.0553923625681914</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L58" s="24" t="n">
+        <f aca="false">L38*L48</f>
+        <v>0.066</v>
+      </c>
+      <c r="M58" s="24" t="n">
+        <f aca="false">M38*M48</f>
+        <v>0.066</v>
+      </c>
+      <c r="N58" s="24" t="n">
+        <f aca="false">N38*N48</f>
+        <v>0.0654637012169534</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L59" s="24" t="n">
+        <f aca="false">L39*L49</f>
+        <v>0.077</v>
+      </c>
+      <c r="M59" s="24" t="n">
+        <f aca="false">M39*M49</f>
+        <v>0.077</v>
+      </c>
+      <c r="N59" s="24" t="n">
+        <f aca="false">N39*N49</f>
+        <v>0.0755350398657155</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L60" s="24" t="n">
+        <f aca="false">L40*L50</f>
+        <v>0.032</v>
+      </c>
+      <c r="M60" s="24" t="n">
+        <f aca="false">M40*M50</f>
+        <v>0.032</v>
+      </c>
+      <c r="N60" s="24" t="n">
+        <f aca="false">N40*N50</f>
+        <v>0.0303189257238775</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K61" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <f aca="false">SUM(L56:L60)</f>
+        <v>0.274</v>
+      </c>
+      <c r="M61" s="0" t="n">
+        <f aca="false">SUM(M56:M60)</f>
+        <v>0.274</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <f aca="false">SUM(N53:N60)</f>
+        <v>0.272975241292488</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -10525,13 +9378,1310 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:R46"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <f aca="false">SUM(C2:E9)</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="51" t="n">
+        <f aca="false">C2*2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="52" t="n">
+        <f aca="false">D2+1</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">SUM(L5:N7)</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <f aca="false">C3*2</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="54" t="n">
+        <f aca="false">D3+1</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <f aca="false">C4*2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="54" t="n">
+        <f aca="false">D4+1</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="53" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">C5*2</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="54" t="n">
+        <f aca="false">D5+1</f>
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <f aca="false">SUM(C2:C4)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <f aca="false">SUM(D2:D4)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <f aca="false">SUM(E2:E4)</f>
+        <v>3</v>
+      </c>
+      <c r="P5" s="18" t="e">
+        <f aca="false">LN(L5)*3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q5" s="18" t="e">
+        <f aca="false">LN(M5)*3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="18" t="n">
+        <f aca="false">LN(N5)*3</f>
+        <v>3.29583686600433</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="53" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <f aca="false">C6*2</f>
+        <v>10</v>
+      </c>
+      <c r="E6" s="54" t="n">
+        <f aca="false">D6+1</f>
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <f aca="false">SUM(C5:C8)</f>
+        <v>22</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <f aca="false">SUM(D5:D8)</f>
+        <v>44</v>
+      </c>
+      <c r="N6" s="8" t="n">
+        <f aca="false">SUM(E5:E8)</f>
+        <v>48</v>
+      </c>
+      <c r="P6" s="59" t="n">
+        <f aca="false">LN(L6)*4</f>
+        <v>12.3641698134333</v>
+      </c>
+      <c r="Q6" s="59" t="n">
+        <f aca="false">LN(M6)*4</f>
+        <v>15.136758535673</v>
+      </c>
+      <c r="R6" s="59" t="n">
+        <f aca="false">LN(N6)*4</f>
+        <v>15.4848040436316</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="53" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <f aca="false">C7*2</f>
+        <v>12</v>
+      </c>
+      <c r="E7" s="54" t="n">
+        <f aca="false">D7+1</f>
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" s="9" t="n">
+        <f aca="false">C9</f>
+        <v>8</v>
+      </c>
+      <c r="M7" s="10" t="n">
+        <f aca="false">D9</f>
+        <v>16</v>
+      </c>
+      <c r="N7" s="11" t="n">
+        <f aca="false">E9</f>
+        <v>17</v>
+      </c>
+      <c r="P7" s="59" t="n">
+        <f aca="false">LN(L7)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="Q7" s="59" t="n">
+        <f aca="false">LN(M7)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="R7" s="59" t="n">
+        <f aca="false">LN(N7)</f>
+        <v>2.83321334405622</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="53" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <f aca="false">C8*2</f>
+        <v>14</v>
+      </c>
+      <c r="E8" s="54" t="n">
+        <f aca="false">D8+1</f>
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" s="58" t="n">
+        <f aca="false">SUM(P6:P7)</f>
+        <v>14.4436113551131</v>
+      </c>
+      <c r="Q8" s="58" t="n">
+        <f aca="false">SUM(Q6:Q7)</f>
+        <v>17.9093472579128</v>
+      </c>
+      <c r="R8" s="58" t="n">
+        <f aca="false">SUM(R6:R7)+R5</f>
+        <v>21.6138542536921</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="55" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="56" t="n">
+        <f aca="false">C9*2</f>
+        <v>16</v>
+      </c>
+      <c r="E9" s="57" t="n">
+        <f aca="false">D9+1</f>
+        <v>17</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="18" t="e">
+        <f aca="false">LN(L5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q10" s="18" t="e">
+        <f aca="false">LN(M5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R10" s="18" t="n">
+        <f aca="false">LN(N5)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" s="18" t="n">
+        <f aca="false">LN(L6)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="Q11" s="18" t="n">
+        <f aca="false">LN(M6)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="R11" s="18" t="n">
+        <f aca="false">LN(N6)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="13" t="e">
+        <f aca="false">LN(C2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D12" s="13" t="e">
+        <f aca="false">LN(D2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="13" t="n">
+        <f aca="false">LN(E2)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="7" t="n">
+        <f aca="false">L5</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="7" t="n">
+        <f aca="false">M5</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="7" t="n">
+        <f aca="false">N5</f>
+        <v>3</v>
+      </c>
+      <c r="P12" s="18" t="n">
+        <f aca="false">LN(L7)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="Q12" s="18" t="n">
+        <f aca="false">LN(M7)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="R12" s="18" t="n">
+        <f aca="false">LN(N7)</f>
+        <v>2.83321334405622</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="13" t="e">
+        <f aca="false">LN(C3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" s="13" t="e">
+        <f aca="false">LN(D3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E13" s="13" t="n">
+        <f aca="false">LN(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="15" t="e">
+        <f aca="false">SUM(C12:E19)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7" t="n">
+        <f aca="false">L12</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="7" t="n">
+        <f aca="false">M12</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="7" t="n">
+        <f aca="false">N12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="13" t="e">
+        <f aca="false">LN(C4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" s="13" t="e">
+        <f aca="false">LN(D4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="13" t="n">
+        <f aca="false">LN(E4)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="58" t="n">
+        <f aca="false">SUM(C15:E19)</f>
+        <v>33.7927555225887</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <f aca="false">L13</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="7" t="n">
+        <f aca="false">M13</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="7" t="n">
+        <f aca="false">N13</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="13" t="n">
+        <f aca="false">LN(C5)</f>
+        <v>1.38629436111989</v>
+      </c>
+      <c r="D15" s="13" t="n">
+        <f aca="false">LN(D5)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="E15" s="13" t="n">
+        <f aca="false">LN(E5)</f>
+        <v>2.19722457733622</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L15" s="7" t="n">
+        <f aca="false">L6</f>
+        <v>22</v>
+      </c>
+      <c r="M15" s="7" t="n">
+        <f aca="false">M6</f>
+        <v>44</v>
+      </c>
+      <c r="N15" s="7" t="n">
+        <f aca="false">N6</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="13" t="n">
+        <f aca="false">LN(C6)</f>
+        <v>1.6094379124341</v>
+      </c>
+      <c r="D16" s="13" t="n">
+        <f aca="false">LN(D6)</f>
+        <v>2.30258509299405</v>
+      </c>
+      <c r="E16" s="13" t="n">
+        <f aca="false">LN(E6)</f>
+        <v>2.39789527279837</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L16" s="7" t="n">
+        <f aca="false">L15</f>
+        <v>22</v>
+      </c>
+      <c r="M16" s="7" t="n">
+        <f aca="false">M15</f>
+        <v>44</v>
+      </c>
+      <c r="N16" s="7" t="n">
+        <f aca="false">N15</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="13" t="n">
+        <f aca="false">LN(C7)</f>
+        <v>1.79175946922806</v>
+      </c>
+      <c r="D17" s="13" t="n">
+        <f aca="false">LN(D7)</f>
+        <v>2.484906649788</v>
+      </c>
+      <c r="E17" s="13" t="n">
+        <f aca="false">LN(E7)</f>
+        <v>2.56494935746154</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L17" s="7" t="n">
+        <f aca="false">L16</f>
+        <v>22</v>
+      </c>
+      <c r="M17" s="7" t="n">
+        <f aca="false">M16</f>
+        <v>44</v>
+      </c>
+      <c r="N17" s="7" t="n">
+        <f aca="false">N16</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="13" t="n">
+        <f aca="false">LN(C8)</f>
+        <v>1.94591014905531</v>
+      </c>
+      <c r="D18" s="13" t="n">
+        <f aca="false">LN(D8)</f>
+        <v>2.63905732961526</v>
+      </c>
+      <c r="E18" s="13" t="n">
+        <f aca="false">LN(E8)</f>
+        <v>2.70805020110221</v>
+      </c>
+      <c r="G18" s="17" t="e">
+        <f aca="false">G13+G25+G32</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L18" s="7" t="n">
+        <f aca="false">L17</f>
+        <v>22</v>
+      </c>
+      <c r="M18" s="7" t="n">
+        <f aca="false">M17</f>
+        <v>44</v>
+      </c>
+      <c r="N18" s="7" t="n">
+        <f aca="false">N17</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="13" t="n">
+        <f aca="false">LN(C9)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="D19" s="13" t="n">
+        <f aca="false">LN(D9)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="E19" s="13" t="n">
+        <f aca="false">LN(E9)</f>
+        <v>2.83321334405622</v>
+      </c>
+      <c r="G19" s="58" t="n">
+        <f aca="false">G14+G27-H34</f>
+        <v>-118.244504558075</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" s="7" t="n">
+        <f aca="false">L7</f>
+        <v>8</v>
+      </c>
+      <c r="M19" s="7" t="n">
+        <f aca="false">M7</f>
+        <v>16</v>
+      </c>
+      <c r="N19" s="7" t="n">
+        <f aca="false">N7</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="J21" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="13" t="e">
+        <f aca="false">LN(L12)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M23" s="13" t="e">
+        <f aca="false">LN(M12)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N23" s="13" t="n">
+        <f aca="false">LN(N12)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="K24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L24" s="13" t="e">
+        <f aca="false">LN(L13)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M24" s="13" t="e">
+        <f aca="false">LN(M13)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N24" s="13" t="n">
+        <f aca="false">LN(N13)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="15" t="e">
+        <f aca="false">SUM(L23:N30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L25" s="13" t="e">
+        <f aca="false">LN(L14)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M25" s="13" t="e">
+        <f aca="false">LN(M14)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N25" s="13" t="n">
+        <f aca="false">LN(N14)</f>
+        <v>1.09861228866811</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="18" t="e">
+        <f aca="false">SUM(P5:R7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L26" s="13" t="n">
+        <f aca="false">LN(L15)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M26" s="13" t="n">
+        <f aca="false">LN(M15)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N26" s="13" t="n">
+        <f aca="false">LN(N15)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="58" t="n">
+        <f aca="false">SUM(P6:R7,R5)</f>
+        <v>53.966812866718</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L27" s="13" t="n">
+        <f aca="false">LN(L16)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M27" s="13" t="n">
+        <f aca="false">LN(M16)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N27" s="13" t="n">
+        <f aca="false">LN(N16)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L28" s="13" t="n">
+        <f aca="false">LN(L17)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M28" s="13" t="n">
+        <f aca="false">LN(M17)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N28" s="13" t="n">
+        <f aca="false">LN(N17)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="n">
+        <f aca="false">L12^2</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">M12^2</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <f aca="false">N12^2</f>
+        <v>9</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L29" s="13" t="n">
+        <f aca="false">LN(L18)</f>
+        <v>3.09104245335832</v>
+      </c>
+      <c r="M29" s="13" t="n">
+        <f aca="false">LN(M18)</f>
+        <v>3.78418963391826</v>
+      </c>
+      <c r="N29" s="13" t="n">
+        <f aca="false">LN(N18)</f>
+        <v>3.87120101090789</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="n">
+        <f aca="false">L13^2</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">M13^2</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <f aca="false">N13^2</f>
+        <v>9</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L30" s="13" t="n">
+        <f aca="false">LN(L19)</f>
+        <v>2.07944154167984</v>
+      </c>
+      <c r="M30" s="13" t="n">
+        <f aca="false">LN(M19)</f>
+        <v>2.77258872223978</v>
+      </c>
+      <c r="N30" s="13" t="n">
+        <f aca="false">LN(N19)</f>
+        <v>2.83321334405622</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="n">
+        <f aca="false">L14^2</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">M14^2</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">N14^2</f>
+        <v>9</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="n">
+        <f aca="false">L15^2</f>
+        <v>484</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="false">M15^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <f aca="false">N15^2</f>
+        <v>2304</v>
+      </c>
+      <c r="G32" s="15" t="n">
+        <f aca="false">SUM(H39:J46)</f>
+        <v>206.004072947381</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="n">
+        <f aca="false">L16^2</f>
+        <v>484</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <f aca="false">M16^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <f aca="false">N16^2</f>
+        <v>2304</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="18" t="n">
+        <f aca="false">SUM(H39:J39)*8</f>
+        <v>206.004072947381</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="0" t="n">
+        <f aca="false">L17^2</f>
+        <v>484</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">M17^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <f aca="false">N17^2</f>
+        <v>2304</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="58" t="n">
+        <f aca="false">SUM(P38:R38)*8</f>
+        <v>206.004072947381</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <f aca="false">L5^2*3</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <f aca="false">M5^2*3</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <f aca="false">N5^2*3</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="n">
+        <f aca="false">L18^2</f>
+        <v>484</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">M18^2</f>
+        <v>1936</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <f aca="false">N18^2</f>
+        <v>2304</v>
+      </c>
+      <c r="P35" s="1" t="n">
+        <f aca="false">L6^2*4</f>
+        <v>1936</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <f aca="false">M6^2*4</f>
+        <v>7744</v>
+      </c>
+      <c r="R35" s="1" t="n">
+        <f aca="false">N6^2*4</f>
+        <v>9216</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="n">
+        <f aca="false">L19^2</f>
+        <v>64</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">M19^2</f>
+        <v>256</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">N19^2</f>
+        <v>289</v>
+      </c>
+      <c r="P36" s="1" t="n">
+        <f aca="false">L7^2</f>
+        <v>64</v>
+      </c>
+      <c r="Q36" s="1" t="n">
+        <f aca="false">M7^2</f>
+        <v>256</v>
+      </c>
+      <c r="R36" s="1" t="n">
+        <f aca="false">N7^2</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="P38" s="0" t="n">
+        <f aca="false">LN(SUM(P34:P36))</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <f aca="false">LN(SUM(Q34:Q36))</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="R38" s="1" t="n">
+        <f aca="false">LN(SUM(R34:R36))</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" s="18" t="n">
+        <f aca="false">LN(C39)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I39" s="18" t="n">
+        <f aca="false">LN(D39)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J39" s="18" t="n">
+        <f aca="false">LN(E39)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" s="18" t="n">
+        <f aca="false">LN(C40)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I40" s="18" t="n">
+        <f aca="false">LN(D40)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J40" s="18" t="n">
+        <f aca="false">LN(E40)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H41" s="18" t="n">
+        <f aca="false">LN(C41)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I41" s="18" t="n">
+        <f aca="false">LN(D41)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J41" s="18" t="n">
+        <f aca="false">LN(E41)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" s="18" t="n">
+        <f aca="false">LN(C42)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I42" s="18" t="n">
+        <f aca="false">LN(D42)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J42" s="18" t="n">
+        <f aca="false">LN(E42)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H43" s="18" t="n">
+        <f aca="false">LN(C43)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I43" s="18" t="n">
+        <f aca="false">LN(D43)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J43" s="18" t="n">
+        <f aca="false">LN(E43)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H44" s="18" t="n">
+        <f aca="false">LN(C44)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I44" s="18" t="n">
+        <f aca="false">LN(D44)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J44" s="18" t="n">
+        <f aca="false">LN(E44)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H45" s="18" t="n">
+        <f aca="false">LN(C45)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I45" s="18" t="n">
+        <f aca="false">LN(D45)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J45" s="18" t="n">
+        <f aca="false">LN(E45)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <f aca="false">SUM(C$29:C$36)</f>
+        <v>2000</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <f aca="false">SUM(D$29:D$36)</f>
+        <v>8000</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <f aca="false">SUM(E$29:E$36)</f>
+        <v>9532</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H46" s="18" t="n">
+        <f aca="false">LN(C46)</f>
+        <v>7.60090245954208</v>
+      </c>
+      <c r="I46" s="18" t="n">
+        <f aca="false">LN(D46)</f>
+        <v>8.98719682066197</v>
+      </c>
+      <c r="J46" s="18" t="n">
+        <f aca="false">LN(E46)</f>
+        <v>9.16240983821863</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="I93:K100 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">

</xml_diff>

<commit_message>
torch mle minor updates
</commit_message>
<xml_diff>
--- a/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
+++ b/Code/MarketPower/nested_logit_MLE_toy_model.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="55">
   <si>
     <t xml:space="preserve">J / iota</t>
   </si>
@@ -132,6 +132,9 @@
     <t xml:space="preserve">product</t>
   </si>
   <si>
+    <t xml:space="preserve">Testing for Normalization (to avoid infinity values in the probabilty computation)</t>
+  </si>
+  <si>
     <t xml:space="preserve">z_\g\i^((1+theta)/(1+eta)) = </t>
   </si>
   <si>
@@ -139,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">denom1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diff</t>
   </si>
   <si>
     <t xml:space="preserve">num2</t>
@@ -1009,11 +1015,11 @@
   </sheetPr>
   <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H61" activeCellId="0" sqref="H61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -2492,16 +2498,16 @@
         <v>1</v>
       </c>
       <c r="C49" s="0" t="n">
-        <f aca="false">C2^($H$48+1)</f>
-        <v>0.0800942345137893</v>
+        <f aca="false">(C2/$H$61)^($H$48+1)</f>
+        <v>0.000253280208511243</v>
       </c>
       <c r="D49" s="0" t="n">
-        <f aca="false">D2^($H$48+1)</f>
-        <v>0.21635247399238</v>
+        <f aca="false">(D2/$H$61)^($H$48+1)</f>
+        <v>0.000684166595228265</v>
       </c>
       <c r="E49" s="0" t="n">
-        <f aca="false">E2^($H$48+1)</f>
-        <v>0.460741381734758</v>
+        <f aca="false">(E2/$H$61)^($H$48+1)</f>
+        <v>0.00145699217857494</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>0</v>
@@ -2534,16 +2540,16 @@
         <v>2</v>
       </c>
       <c r="C50" s="0" t="n">
-        <f aca="false">C3^($H$48+1)</f>
-        <v>0.421461130645012</v>
+        <f aca="false">(C3/$H$61)^($H$48+1)</f>
+        <v>0.00133277711806803</v>
       </c>
       <c r="D50" s="0" t="n">
-        <f aca="false">D3^($H$48+1)</f>
-        <v>0.099624626168005</v>
+        <f aca="false">(D3/$H$61)^($H$48+1)</f>
+        <v>0.000315040729733708</v>
       </c>
       <c r="E50" s="0" t="n">
-        <f aca="false">E3^($H$48+1)</f>
-        <v>0.428920426825316</v>
+        <f aca="false">(E3/$H$61)^($H$48+1)</f>
+        <v>0.00135636548373958</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>1</v>
@@ -2567,16 +2573,16 @@
         <v>3</v>
       </c>
       <c r="C51" s="0" t="n">
-        <f aca="false">C4^($H$48+1)</f>
-        <v>0.0609051604367493</v>
+        <f aca="false">(C4/$H$61)^($H$48+1)</f>
+        <v>0.000192599028238103</v>
       </c>
       <c r="D51" s="0" t="n">
-        <f aca="false">D4^($H$48+1)</f>
-        <v>0.110974543892054</v>
+        <f aca="false">(D4/$H$61)^($H$48+1)</f>
+        <v>0.000350932320997219</v>
       </c>
       <c r="E51" s="0" t="n">
-        <f aca="false">E4^($H$48+1)</f>
-        <v>0.564913850136054</v>
+        <f aca="false">(E4/$H$61)^($H$48+1)</f>
+        <v>0.00178641444820495</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>2</v>
@@ -2603,16 +2609,16 @@
         <v>4</v>
       </c>
       <c r="C52" s="0" t="n">
-        <f aca="false">C5^($H$48+1)</f>
-        <v>0.362130316253291</v>
+        <f aca="false">(C5/$H$61)^($H$48+1)</f>
+        <v>0.00114515660915749</v>
       </c>
       <c r="D52" s="0" t="n">
-        <f aca="false">D5^($H$48+1)</f>
-        <v>0.0689503003711744</v>
+        <f aca="false">(D5/$H$61)^($H$48+1)</f>
+        <v>0.000218039994525664</v>
       </c>
       <c r="E52" s="0" t="n">
-        <f aca="false">E5^($H$48+1)</f>
-        <v>0.0250696298255445</v>
+        <f aca="false">(E5/$H$61)^($H$48+1)</f>
+        <v>7.92771303460103E-005</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>0</v>
@@ -2629,16 +2635,16 @@
         <v>5</v>
       </c>
       <c r="C53" s="0" t="n">
-        <f aca="false">C6^($H$48+1)</f>
-        <v>0.0016799044275743</v>
+        <f aca="false">(C6/$H$61)^($H$48+1)</f>
+        <v>5.31232424253617E-006</v>
       </c>
       <c r="D53" s="0" t="n">
-        <f aca="false">D6^($H$48+1)</f>
-        <v>0.0779917047976806</v>
+        <f aca="false">(D6/$H$61)^($H$48+1)</f>
+        <v>0.000246631425760152</v>
       </c>
       <c r="E53" s="0" t="n">
-        <f aca="false">E6^($H$48+1)</f>
-        <v>0.0101332048083469</v>
+        <f aca="false">(E6/$H$61)^($H$48+1)</f>
+        <v>3.20440071913461E-005</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>2</v>
@@ -2662,16 +2668,16 @@
         <v>6</v>
       </c>
       <c r="C54" s="0" t="n">
-        <f aca="false">C7^($H$48+1)</f>
-        <v>0.00222813658443647</v>
+        <f aca="false">(C7/$H$61)^($H$48+1)</f>
+        <v>7.04598654476733E-006</v>
       </c>
       <c r="D54" s="0" t="n">
-        <f aca="false">D7^($H$48+1)</f>
-        <v>0.050811953771441</v>
+        <f aca="false">(D7/$H$61)^($H$48+1)</f>
+        <v>0.000160681506280936</v>
       </c>
       <c r="E54" s="0" t="n">
-        <f aca="false">E7^($H$48+1)</f>
-        <v>0.109541598592283</v>
+        <f aca="false">(E7/$H$61)^($H$48+1)</f>
+        <v>0.000346400950087509</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>0</v>
@@ -2695,16 +2701,16 @@
         <v>7</v>
       </c>
       <c r="C55" s="0" t="n">
-        <f aca="false">C8^($H$48+1)</f>
-        <v>0.108772351507056</v>
+        <f aca="false">(C8/$H$61)^($H$48+1)</f>
+        <v>0.000343968377214747</v>
       </c>
       <c r="D55" s="0" t="n">
-        <f aca="false">D8^($H$48+1)</f>
-        <v>0.968695747337174</v>
+        <f aca="false">(D8/$H$61)^($H$48+1)</f>
+        <v>0.00306328492130446</v>
       </c>
       <c r="E55" s="0" t="n">
-        <f aca="false">E8^($H$48+1)</f>
-        <v>0.115172796908422</v>
+        <f aca="false">(E8/$H$61)^($H$48+1)</f>
+        <v>0.000364208362722613</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>2</v>
@@ -2728,16 +2734,16 @@
         <v>8</v>
       </c>
       <c r="C56" s="0" t="n">
-        <f aca="false">C9^($H$48+1)</f>
-        <v>0.0421583946420825</v>
+        <f aca="false">(C9/$H$61)^($H$48+1)</f>
+        <v>0.00013331654956522</v>
       </c>
       <c r="D56" s="0" t="n">
-        <f aca="false">D9^($H$48+1)</f>
-        <v>0.302628412296439</v>
+        <f aca="false">(D9/$H$61)^($H$48+1)</f>
+        <v>0.000956995067537254</v>
       </c>
       <c r="E56" s="0" t="n">
-        <f aca="false">E9^($H$48+1)</f>
-        <v>0.339010781284527</v>
+        <f aca="false">(E9/$H$61)^($H$48+1)</f>
+        <v>0.00107204622021229</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>2</v>
@@ -2817,6 +2823,9 @@
       <c r="E60" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="H60" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="J60" s="23"/>
       <c r="L60" s="25" t="n">
         <f aca="false">L40*L50</f>
@@ -2837,15 +2846,18 @@
       </c>
       <c r="C61" s="3" t="n">
         <f aca="false">C49+C52+C54</f>
-        <v>0.444452687351517</v>
+        <v>0.0014054828042135</v>
       </c>
       <c r="D61" s="3" t="n">
         <f aca="false">D49+D52+D54</f>
-        <v>0.336114728134996</v>
+        <v>0.00106288809603487</v>
       </c>
       <c r="E61" s="3" t="n">
         <f aca="false">E49+E52+E54</f>
-        <v>0.595352610152585</v>
+        <v>0.00188267025900845</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>10</v>
       </c>
       <c r="J61" s="23"/>
       <c r="K61" s="21" t="s">
@@ -2870,15 +2882,15 @@
       </c>
       <c r="C62" s="6" t="n">
         <f aca="false">C50</f>
-        <v>0.421461130645012</v>
+        <v>0.00133277711806803</v>
       </c>
       <c r="D62" s="6" t="n">
         <f aca="false">D50</f>
-        <v>0.099624626168005</v>
+        <v>0.000315040729733708</v>
       </c>
       <c r="E62" s="6" t="n">
         <f aca="false">E50</f>
-        <v>0.428920426825316</v>
+        <v>0.00135636548373958</v>
       </c>
       <c r="J62" s="23"/>
     </row>
@@ -2888,15 +2900,15 @@
       </c>
       <c r="C63" s="9" t="n">
         <f aca="false">C51+C53+C55+C56</f>
-        <v>0.213515811013462</v>
+        <v>0.000675196279260606</v>
       </c>
       <c r="D63" s="9" t="n">
         <f aca="false">D51+D53+D55+D56</f>
-        <v>1.46029040832335</v>
+        <v>0.00461784373559908</v>
       </c>
       <c r="E63" s="9" t="n">
         <f aca="false">E51+E53+E55+E56</f>
-        <v>1.02923063313735</v>
+        <v>0.0032547130383312</v>
       </c>
       <c r="J63" s="23"/>
     </row>
@@ -2905,7 +2917,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J65" s="23"/>
     </row>
@@ -2930,15 +2942,15 @@
       </c>
       <c r="C67" s="3" t="n">
         <f aca="false">C61^((1+$H$49)/(1+$H$48))</f>
-        <v>0.614745448393954</v>
+        <v>0.0194399579814639</v>
       </c>
       <c r="D67" s="3" t="n">
         <f aca="false">D61^((1+$H$49)/(1+$H$48))</f>
-        <v>0.51986732992912</v>
+        <v>0.0164396484368624</v>
       </c>
       <c r="E67" s="3" t="n">
         <f aca="false">E61^((1+$H$49)/(1+$H$48))</f>
-        <v>0.732596023838905</v>
+        <v>0.0231667204011395</v>
       </c>
       <c r="J67" s="23"/>
     </row>
@@ -2948,15 +2960,15 @@
       </c>
       <c r="C68" s="3" t="n">
         <f aca="false">C62^((1+$H$49)/(1+$H$48))</f>
-        <v>0.595462637518301</v>
+        <v>0.0188301819608906</v>
       </c>
       <c r="D68" s="3" t="n">
         <f aca="false">D62^((1+$H$49)/(1+$H$48))</f>
-        <v>0.250622479817689</v>
+        <v>0.00792537869063478</v>
       </c>
       <c r="E68" s="3" t="n">
         <f aca="false">E62^((1+$H$49)/(1+$H$48))</f>
-        <v>0.601763771092214</v>
+        <v>0.0190294413002359</v>
       </c>
       <c r="J68" s="23"/>
     </row>
@@ -2966,15 +2978,15 @@
       </c>
       <c r="C69" s="3" t="n">
         <f aca="false">C63^((1+$H$49)/(1+$H$48))</f>
-        <v>0.395966116543806</v>
+        <v>0.0125215480453011</v>
       </c>
       <c r="D69" s="3" t="n">
         <f aca="false">D63^((1+$H$49)/(1+$H$48))</f>
-        <v>1.25505725800389</v>
+        <v>0.039688395292179</v>
       </c>
       <c r="E69" s="3" t="n">
         <f aca="false">E63^((1+$H$49)/(1+$H$48))</f>
-        <v>1.01743722286996</v>
+        <v>0.0321741900050544</v>
       </c>
       <c r="J69" s="23"/>
     </row>
@@ -2984,15 +2996,15 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="n">
         <f aca="false">SUM(C67:C69)</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">SUM(D67:D69)</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="E71" s="0" t="n">
         <f aca="false">SUM(E67:E69)</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J71" s="23"/>
     </row>
@@ -3001,10 +3013,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J73" s="23"/>
     </row>
@@ -3014,27 +3026,27 @@
       </c>
       <c r="C74" s="0" t="n">
         <f aca="false">C61</f>
-        <v>0.444452687351517</v>
+        <v>0.0014054828042135</v>
       </c>
       <c r="D74" s="0" t="n">
         <f aca="false">D61</f>
-        <v>0.336114728134996</v>
+        <v>0.00106288809603487</v>
       </c>
       <c r="E74" s="0" t="n">
         <f aca="false">E61</f>
-        <v>0.595352610152585</v>
+        <v>0.00188267025900845</v>
       </c>
       <c r="F74" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G74" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H74" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J74" s="23"/>
     </row>
@@ -3044,27 +3056,27 @@
       </c>
       <c r="C75" s="0" t="n">
         <f aca="false">C62</f>
-        <v>0.421461130645012</v>
+        <v>0.00133277711806803</v>
       </c>
       <c r="D75" s="0" t="n">
         <f aca="false">D62</f>
-        <v>0.099624626168005</v>
+        <v>0.000315040729733708</v>
       </c>
       <c r="E75" s="0" t="n">
         <f aca="false">E62</f>
-        <v>0.428920426825316</v>
+        <v>0.00135636548373958</v>
       </c>
       <c r="F75" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G75" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H75" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J75" s="23"/>
     </row>
@@ -3074,27 +3086,27 @@
       </c>
       <c r="C76" s="0" t="n">
         <f aca="false">C63</f>
-        <v>0.213515811013462</v>
+        <v>0.000675196279260606</v>
       </c>
       <c r="D76" s="0" t="n">
         <f aca="false">D63</f>
-        <v>1.46029040832335</v>
+        <v>0.00461784373559908</v>
       </c>
       <c r="E76" s="0" t="n">
         <f aca="false">E63</f>
-        <v>1.02923063313735</v>
+        <v>0.0032547130383312</v>
       </c>
       <c r="F76" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G76" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H76" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J76" s="23"/>
     </row>
@@ -3104,27 +3116,27 @@
       </c>
       <c r="C77" s="0" t="n">
         <f aca="false">C61</f>
-        <v>0.444452687351517</v>
+        <v>0.0014054828042135</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">D61</f>
-        <v>0.336114728134996</v>
+        <v>0.00106288809603487</v>
       </c>
       <c r="E77" s="0" t="n">
         <f aca="false">E61</f>
-        <v>0.595352610152585</v>
+        <v>0.00188267025900845</v>
       </c>
       <c r="F77" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G77" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H77" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J77" s="23"/>
     </row>
@@ -3134,27 +3146,27 @@
       </c>
       <c r="C78" s="0" t="n">
         <f aca="false">C63</f>
-        <v>0.213515811013462</v>
+        <v>0.000675196279260606</v>
       </c>
       <c r="D78" s="0" t="n">
         <f aca="false">D63</f>
-        <v>1.46029040832335</v>
+        <v>0.00461784373559908</v>
       </c>
       <c r="E78" s="0" t="n">
         <f aca="false">E63</f>
-        <v>1.02923063313735</v>
+        <v>0.0032547130383312</v>
       </c>
       <c r="F78" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G78" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H78" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J78" s="23"/>
     </row>
@@ -3164,29 +3176,32 @@
       </c>
       <c r="C79" s="0" t="n">
         <f aca="false">C61</f>
-        <v>0.444452687351517</v>
+        <v>0.0014054828042135</v>
       </c>
       <c r="D79" s="0" t="n">
         <f aca="false">D61</f>
-        <v>0.336114728134996</v>
+        <v>0.00106288809603487</v>
       </c>
       <c r="E79" s="0" t="n">
         <f aca="false">E61</f>
-        <v>0.595352610152585</v>
+        <v>0.00188267025900845</v>
       </c>
       <c r="F79" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G79" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H79" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J79" s="23"/>
+      <c r="O79" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="n">
@@ -3194,32 +3209,44 @@
       </c>
       <c r="C80" s="0" t="n">
         <f aca="false">C63</f>
-        <v>0.213515811013462</v>
+        <v>0.000675196279260606</v>
       </c>
       <c r="D80" s="0" t="n">
         <f aca="false">D63</f>
-        <v>1.46029040832335</v>
+        <v>0.00461784373559908</v>
       </c>
       <c r="E80" s="0" t="n">
         <f aca="false">E63</f>
-        <v>1.02923063313735</v>
+        <v>0.0032547130383312</v>
       </c>
       <c r="F80" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G80" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H80" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="J80" s="23"/>
       <c r="K80" s="22"/>
       <c r="L80" s="22"/>
       <c r="M80" s="22"/>
+      <c r="O80" s="0" t="n">
+        <f aca="false">I93-O93</f>
+        <v>0</v>
+      </c>
+      <c r="P80" s="0" t="n">
+        <f aca="false">J93-P93</f>
+        <v>0</v>
+      </c>
+      <c r="Q80" s="0" t="n">
+        <f aca="false">K93-Q93</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="n">
@@ -3227,38 +3254,62 @@
       </c>
       <c r="C81" s="0" t="n">
         <f aca="false">C63</f>
-        <v>0.213515811013462</v>
+        <v>0.000675196279260606</v>
       </c>
       <c r="D81" s="0" t="n">
         <f aca="false">D63</f>
-        <v>1.46029040832335</v>
+        <v>0.00461784373559908</v>
       </c>
       <c r="E81" s="0" t="n">
         <f aca="false">E63</f>
-        <v>1.02923063313735</v>
+        <v>0.0032547130383312</v>
       </c>
       <c r="F81" s="0" t="n">
         <f aca="false">C$71</f>
-        <v>1.60617420245606</v>
+        <v>0.0507916879876557</v>
       </c>
       <c r="G81" s="0" t="n">
         <f aca="false">D$71</f>
-        <v>2.0255470677507</v>
+        <v>0.0640534224196762</v>
       </c>
       <c r="H81" s="0" t="n">
         <f aca="false">E$71</f>
-        <v>2.35179701780108</v>
+        <v>0.0743703517064298</v>
       </c>
       <c r="M81" s="22"/>
+      <c r="O81" s="0" t="n">
+        <f aca="false">I94-O94</f>
+        <v>0</v>
+      </c>
+      <c r="P81" s="0" t="n">
+        <f aca="false">J94-P94</f>
+        <v>0</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <f aca="false">K94-Q94</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M82" s="22"/>
+      <c r="O82" s="0" t="n">
+        <f aca="false">I95-O95</f>
+        <v>0</v>
+      </c>
+      <c r="P82" s="0" t="n">
+        <f aca="false">J95-P95</f>
+        <v>0</v>
+      </c>
+      <c r="Q82" s="0" t="n">
+        <f aca="false">K95-Q95</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="n">
@@ -3266,29 +3317,41 @@
       </c>
       <c r="C83" s="0" t="n">
         <f aca="false">C49</f>
-        <v>0.0800942345137893</v>
+        <v>0.000253280208511243</v>
       </c>
       <c r="D83" s="0" t="n">
         <f aca="false">D49</f>
-        <v>0.21635247399238</v>
+        <v>0.000684166595228265</v>
       </c>
       <c r="E83" s="0" t="n">
         <f aca="false">E49</f>
-        <v>0.460741381734758</v>
+        <v>0.00145699217857494</v>
       </c>
       <c r="F83" s="0" t="n">
         <f aca="false">C67</f>
-        <v>0.614745448393954</v>
+        <v>0.0194399579814639</v>
       </c>
       <c r="G83" s="0" t="n">
         <f aca="false">D67</f>
-        <v>0.51986732992912</v>
+        <v>0.0164396484368624</v>
       </c>
       <c r="H83" s="0" t="n">
         <f aca="false">E67</f>
-        <v>0.732596023838905</v>
+        <v>0.0231667204011395</v>
       </c>
       <c r="M83" s="22"/>
+      <c r="O83" s="0" t="n">
+        <f aca="false">I96-O96</f>
+        <v>0</v>
+      </c>
+      <c r="P83" s="0" t="n">
+        <f aca="false">J96-P96</f>
+        <v>0</v>
+      </c>
+      <c r="Q83" s="0" t="n">
+        <f aca="false">K96-Q96</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="n">
@@ -3296,29 +3359,41 @@
       </c>
       <c r="C84" s="0" t="n">
         <f aca="false">C50</f>
-        <v>0.421461130645012</v>
+        <v>0.00133277711806803</v>
       </c>
       <c r="D84" s="0" t="n">
         <f aca="false">D50</f>
-        <v>0.099624626168005</v>
+        <v>0.000315040729733708</v>
       </c>
       <c r="E84" s="0" t="n">
         <f aca="false">E50</f>
-        <v>0.428920426825316</v>
+        <v>0.00135636548373958</v>
       </c>
       <c r="F84" s="0" t="n">
         <f aca="false">C68</f>
-        <v>0.595462637518301</v>
+        <v>0.0188301819608906</v>
       </c>
       <c r="G84" s="0" t="n">
         <f aca="false">D68</f>
-        <v>0.250622479817689</v>
+        <v>0.00792537869063478</v>
       </c>
       <c r="H84" s="0" t="n">
         <f aca="false">E68</f>
-        <v>0.601763771092214</v>
+        <v>0.0190294413002359</v>
       </c>
       <c r="M84" s="22"/>
+      <c r="O84" s="0" t="n">
+        <f aca="false">I97-O97</f>
+        <v>0</v>
+      </c>
+      <c r="P84" s="0" t="n">
+        <f aca="false">J97-P97</f>
+        <v>0</v>
+      </c>
+      <c r="Q84" s="0" t="n">
+        <f aca="false">K97-Q97</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="n">
@@ -3326,29 +3401,41 @@
       </c>
       <c r="C85" s="0" t="n">
         <f aca="false">C51</f>
-        <v>0.0609051604367493</v>
+        <v>0.000192599028238103</v>
       </c>
       <c r="D85" s="0" t="n">
         <f aca="false">D51</f>
-        <v>0.110974543892054</v>
+        <v>0.000350932320997219</v>
       </c>
       <c r="E85" s="0" t="n">
         <f aca="false">E51</f>
-        <v>0.564913850136054</v>
+        <v>0.00178641444820495</v>
       </c>
       <c r="F85" s="0" t="n">
         <f aca="false">C69</f>
-        <v>0.395966116543806</v>
+        <v>0.0125215480453011</v>
       </c>
       <c r="G85" s="0" t="n">
         <f aca="false">D69</f>
-        <v>1.25505725800389</v>
+        <v>0.039688395292179</v>
       </c>
       <c r="H85" s="0" t="n">
         <f aca="false">E69</f>
-        <v>1.01743722286996</v>
+        <v>0.0321741900050544</v>
       </c>
       <c r="M85" s="22"/>
+      <c r="O85" s="0" t="n">
+        <f aca="false">I98-O98</f>
+        <v>0</v>
+      </c>
+      <c r="P85" s="0" t="n">
+        <f aca="false">J98-P98</f>
+        <v>0</v>
+      </c>
+      <c r="Q85" s="0" t="n">
+        <f aca="false">K98-Q98</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="n">
@@ -3356,29 +3443,41 @@
       </c>
       <c r="C86" s="0" t="n">
         <f aca="false">C52</f>
-        <v>0.362130316253291</v>
+        <v>0.00114515660915749</v>
       </c>
       <c r="D86" s="0" t="n">
         <f aca="false">D52</f>
-        <v>0.0689503003711744</v>
+        <v>0.000218039994525664</v>
       </c>
       <c r="E86" s="0" t="n">
         <f aca="false">E52</f>
-        <v>0.0250696298255445</v>
+        <v>7.92771303460103E-005</v>
       </c>
       <c r="F86" s="0" t="n">
         <f aca="false">C67</f>
-        <v>0.614745448393954</v>
+        <v>0.0194399579814639</v>
       </c>
       <c r="G86" s="0" t="n">
         <f aca="false">D67</f>
-        <v>0.51986732992912</v>
+        <v>0.0164396484368624</v>
       </c>
       <c r="H86" s="0" t="n">
         <f aca="false">E67</f>
-        <v>0.732596023838905</v>
+        <v>0.0231667204011395</v>
       </c>
       <c r="M86" s="22"/>
+      <c r="O86" s="0" t="n">
+        <f aca="false">I99-O99</f>
+        <v>0</v>
+      </c>
+      <c r="P86" s="0" t="n">
+        <f aca="false">J99-P99</f>
+        <v>0</v>
+      </c>
+      <c r="Q86" s="0" t="n">
+        <f aca="false">K99-Q99</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="n">
@@ -3386,29 +3485,41 @@
       </c>
       <c r="C87" s="0" t="n">
         <f aca="false">C53</f>
-        <v>0.0016799044275743</v>
+        <v>5.31232424253617E-006</v>
       </c>
       <c r="D87" s="0" t="n">
         <f aca="false">D53</f>
-        <v>0.0779917047976806</v>
+        <v>0.000246631425760152</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">E53</f>
-        <v>0.0101332048083469</v>
+        <v>3.20440071913461E-005</v>
       </c>
       <c r="F87" s="0" t="n">
         <f aca="false">C69</f>
-        <v>0.395966116543806</v>
+        <v>0.0125215480453011</v>
       </c>
       <c r="G87" s="0" t="n">
         <f aca="false">D69</f>
-        <v>1.25505725800389</v>
+        <v>0.039688395292179</v>
       </c>
       <c r="H87" s="0" t="n">
         <f aca="false">E69</f>
-        <v>1.01743722286996</v>
+        <v>0.0321741900050544</v>
       </c>
       <c r="M87" s="22"/>
+      <c r="O87" s="0" t="n">
+        <f aca="false">I100-O100</f>
+        <v>0</v>
+      </c>
+      <c r="P87" s="0" t="n">
+        <f aca="false">J100-P100</f>
+        <v>0</v>
+      </c>
+      <c r="Q87" s="0" t="n">
+        <f aca="false">K100-Q100</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="n">
@@ -3416,29 +3527,41 @@
       </c>
       <c r="C88" s="0" t="n">
         <f aca="false">C54</f>
-        <v>0.00222813658443647</v>
+        <v>7.04598654476733E-006</v>
       </c>
       <c r="D88" s="0" t="n">
         <f aca="false">D54</f>
-        <v>0.050811953771441</v>
+        <v>0.000160681506280936</v>
       </c>
       <c r="E88" s="0" t="n">
         <f aca="false">E54</f>
-        <v>0.109541598592283</v>
+        <v>0.000346400950087509</v>
       </c>
       <c r="F88" s="0" t="n">
         <f aca="false">C67</f>
-        <v>0.614745448393954</v>
+        <v>0.0194399579814639</v>
       </c>
       <c r="G88" s="0" t="n">
         <f aca="false">D67</f>
-        <v>0.51986732992912</v>
+        <v>0.0164396484368624</v>
       </c>
       <c r="H88" s="0" t="n">
         <f aca="false">E67</f>
-        <v>0.732596023838905</v>
+        <v>0.0231667204011395</v>
       </c>
       <c r="M88" s="22"/>
+      <c r="O88" s="0" t="n">
+        <f aca="false">I101-O101</f>
+        <v>0</v>
+      </c>
+      <c r="P88" s="0" t="n">
+        <f aca="false">J101-P101</f>
+        <v>0</v>
+      </c>
+      <c r="Q88" s="0" t="n">
+        <f aca="false">K101-Q101</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="n">
@@ -3446,27 +3569,27 @@
       </c>
       <c r="C89" s="0" t="n">
         <f aca="false">C55</f>
-        <v>0.108772351507056</v>
+        <v>0.000343968377214747</v>
       </c>
       <c r="D89" s="0" t="n">
         <f aca="false">D55</f>
-        <v>0.968695747337174</v>
+        <v>0.00306328492130446</v>
       </c>
       <c r="E89" s="0" t="n">
         <f aca="false">E55</f>
-        <v>0.115172796908422</v>
+        <v>0.000364208362722613</v>
       </c>
       <c r="F89" s="0" t="n">
         <f aca="false">C69</f>
-        <v>0.395966116543806</v>
+        <v>0.0125215480453011</v>
       </c>
       <c r="G89" s="0" t="n">
         <f aca="false">D69</f>
-        <v>1.25505725800389</v>
+        <v>0.039688395292179</v>
       </c>
       <c r="H89" s="0" t="n">
         <f aca="false">E69</f>
-        <v>1.01743722286996</v>
+        <v>0.0321741900050544</v>
       </c>
       <c r="M89" s="22"/>
     </row>
@@ -3476,27 +3599,27 @@
       </c>
       <c r="C90" s="0" t="n">
         <f aca="false">C56</f>
-        <v>0.0421583946420825</v>
+        <v>0.00013331654956522</v>
       </c>
       <c r="D90" s="0" t="n">
         <f aca="false">D56</f>
-        <v>0.302628412296439</v>
+        <v>0.000956995067537254</v>
       </c>
       <c r="E90" s="0" t="n">
         <f aca="false">E56</f>
-        <v>0.339010781284527</v>
+        <v>0.00107204622021229</v>
       </c>
       <c r="F90" s="0" t="n">
         <f aca="false">C69</f>
-        <v>0.395966116543806</v>
+        <v>0.0125215480453011</v>
       </c>
       <c r="G90" s="0" t="n">
         <f aca="false">D69</f>
-        <v>1.25505725800389</v>
+        <v>0.039688395292179</v>
       </c>
       <c r="H90" s="0" t="n">
         <f aca="false">E69</f>
-        <v>1.01743722286996</v>
+        <v>0.0321741900050544</v>
       </c>
       <c r="M90" s="22"/>
     </row>
@@ -3505,15 +3628,18 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I92" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M92" s="22"/>
+      <c r="O92" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="n">
@@ -3537,7 +3663,7 @@
       </c>
       <c r="G93" s="0" t="n">
         <f aca="false">G83/G74</f>
-        <v>0.256655270176671</v>
+        <v>0.25665527017667</v>
       </c>
       <c r="H93" s="0" t="n">
         <f aca="false">H83/H74</f>
@@ -3556,6 +3682,15 @@
         <v>0.241072504767219</v>
       </c>
       <c r="M93" s="22"/>
+      <c r="O93" s="26" t="n">
+        <v>0.0689728853485442</v>
+      </c>
+      <c r="P93" s="26" t="n">
+        <v>0.165205502817489</v>
+      </c>
+      <c r="Q93" s="26" t="n">
+        <v>0.241072504767219</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="n">
@@ -3575,7 +3710,7 @@
       </c>
       <c r="F94" s="0" t="n">
         <f aca="false">F84/F75</f>
-        <v>0.370733533515703</v>
+        <v>0.370733533515702</v>
       </c>
       <c r="G94" s="0" t="n">
         <f aca="false">G84/G75</f>
@@ -3587,7 +3722,7 @@
       </c>
       <c r="I94" s="26" t="n">
         <f aca="false">C94*F94</f>
-        <v>0.370733533515703</v>
+        <v>0.370733533515702</v>
       </c>
       <c r="J94" s="26" t="n">
         <f aca="false">D94*G94</f>
@@ -3598,6 +3733,15 @@
         <v>0.255874025920341</v>
       </c>
       <c r="M94" s="22"/>
+      <c r="O94" s="26" t="n">
+        <v>0.370733533515703</v>
+      </c>
+      <c r="P94" s="26" t="n">
+        <v>0.123730760843783</v>
+      </c>
+      <c r="Q94" s="26" t="n">
+        <v>0.255874025920341</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="n">
@@ -3625,7 +3769,7 @@
       </c>
       <c r="H95" s="0" t="n">
         <f aca="false">H85/H76</f>
-        <v>0.432621189315591</v>
+        <v>0.43262118931559</v>
       </c>
       <c r="I95" s="26" t="n">
         <f aca="false">C95*F95</f>
@@ -3640,6 +3784,15 @@
         <v>0.237452805851431</v>
       </c>
       <c r="M95" s="22"/>
+      <c r="O95" s="26" t="n">
+        <v>0.0703217110248094</v>
+      </c>
+      <c r="P95" s="26" t="n">
+        <v>0.0470874678110088</v>
+      </c>
+      <c r="Q95" s="26" t="n">
+        <v>0.237452805851431</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="n">
@@ -3663,7 +3816,7 @@
       </c>
       <c r="G96" s="0" t="n">
         <f aca="false">G86/G77</f>
-        <v>0.256655270176671</v>
+        <v>0.25665527017667</v>
       </c>
       <c r="H96" s="0" t="n">
         <f aca="false">H86/H77</f>
@@ -3682,6 +3835,15 @@
         <v>0.0131171166628792</v>
       </c>
       <c r="M96" s="22"/>
+      <c r="O96" s="26" t="n">
+        <v>0.311847325038985</v>
+      </c>
+      <c r="P96" s="26" t="n">
+        <v>0.0526500521673624</v>
+      </c>
+      <c r="Q96" s="26" t="n">
+        <v>0.0131171166628792</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="n">
@@ -3709,7 +3871,7 @@
       </c>
       <c r="H97" s="0" t="n">
         <f aca="false">H87/H78</f>
-        <v>0.432621189315591</v>
+        <v>0.43262118931559</v>
       </c>
       <c r="I97" s="26" t="n">
         <f aca="false">C97*F97</f>
@@ -3724,6 +3886,15 @@
         <v>0.00425933602695292</v>
       </c>
       <c r="M97" s="22"/>
+      <c r="O97" s="26" t="n">
+        <v>0.00193963455408448</v>
+      </c>
+      <c r="P97" s="26" t="n">
+        <v>0.0330925612342114</v>
+      </c>
+      <c r="Q97" s="26" t="n">
+        <v>0.00425933602695292</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="n">
@@ -3731,7 +3902,7 @@
       </c>
       <c r="C98" s="0" t="n">
         <f aca="false">C88/C79</f>
-        <v>0.00501321433719725</v>
+        <v>0.00501321433719724</v>
       </c>
       <c r="D98" s="0" t="n">
         <f aca="false">D88/D79</f>
@@ -3747,7 +3918,7 @@
       </c>
       <c r="G98" s="0" t="n">
         <f aca="false">G88/G79</f>
-        <v>0.256655270176671</v>
+        <v>0.25665527017667</v>
       </c>
       <c r="H98" s="0" t="n">
         <f aca="false">H88/H79</f>
@@ -3766,6 +3937,15 @@
         <v>0.0573151633339707</v>
       </c>
       <c r="M98" s="22"/>
+      <c r="O98" s="26" t="n">
+        <v>0.00191875245593084</v>
+      </c>
+      <c r="P98" s="26" t="n">
+        <v>0.0387997151918195</v>
+      </c>
+      <c r="Q98" s="26" t="n">
+        <v>0.0573151633339707</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="n">
@@ -3793,7 +3973,7 @@
       </c>
       <c r="H99" s="0" t="n">
         <f aca="false">H89/H80</f>
-        <v>0.432621189315591</v>
+        <v>0.43262118931559</v>
       </c>
       <c r="I99" s="26" t="n">
         <f aca="false">C99*F99</f>
@@ -3808,6 +3988,15 @@
         <v>0.0484111051217373</v>
       </c>
       <c r="M99" s="22"/>
+      <c r="O99" s="26" t="n">
+        <v>0.125589651440322</v>
+      </c>
+      <c r="P99" s="26" t="n">
+        <v>0.411026062569528</v>
+      </c>
+      <c r="Q99" s="26" t="n">
+        <v>0.0484111051217373</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="n">
@@ -3835,7 +4024,7 @@
       </c>
       <c r="H100" s="0" t="n">
         <f aca="false">H90/H81</f>
-        <v>0.432621189315591</v>
+        <v>0.43262118931559</v>
       </c>
       <c r="I100" s="26" t="n">
         <f aca="false">C100*F100</f>
@@ -3850,6 +4039,15 @@
         <v>0.142497942315469</v>
       </c>
       <c r="M100" s="22"/>
+      <c r="O100" s="26" t="n">
+        <v>0.0486765066216224</v>
+      </c>
+      <c r="P100" s="26" t="n">
+        <v>0.128407877364798</v>
+      </c>
+      <c r="Q100" s="26" t="n">
+        <v>0.142497942315469</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M101" s="22"/>
@@ -3939,28 +4137,28 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27"/>
       <c r="B1" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,7 +4205,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B6" s="47" t="n">
         <v>0.999335394496202</v>
@@ -4041,7 +4239,7 @@
       <selection pane="topLeft" activeCell="L53" activeCellId="0" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -5707,7 +5905,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -7385,20 +7583,20 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7559,20 +7757,20 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7709,7 +7907,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -8351,7 +8549,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>0</v>
@@ -8368,7 +8566,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>18</v>
@@ -9384,7 +9582,7 @@
       <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.99"/>
@@ -10026,7 +10224,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K22" s="0" t="s">
         <v>0</v>
@@ -10043,7 +10241,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>18</v>
@@ -10681,20 +10879,20 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="50" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>